<commit_message>
research: Qwen 2.5 실험 결과 추가
</commit_message>
<xml_diff>
--- a/deuChatbot/research_result/results/bleu_score/bleu_version_1(1500_0).xlsx
+++ b/deuChatbot/research_result/results/bleu_score/bleu_version_1(1500_0).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D273"/>
+  <dimension ref="A1:D374"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7731,81 +7731,3365 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>GPT-4o-mini Average</t>
+          <t>Qwen2.5-7B-instruct</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>디자인조형학과의 실기시험에 대한 정보는 다음과 같습니다:
+ 모집단위 및 실기종목
+- 모집단위: 시각디자인, 산업디자인, 공예디자인
+- 실기종목: 기초디자인, 사고의 전환
+종목별 배점(비율)
+- 배점 : 700점 (70%)
+실기종목별 준비물, 실기주제, 화지크기 및 시험시간
+1. 기초디자인
+- 준비물 : 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구
+- 실기주제 : 주제A, 주제B에서 각 1개씩 선정하여 연결된 주제를 당일 추첨 (예시: 잠자리와 저울)
+- 주제A: 잠자리, 무궁화, 피망, 고양이, 양파, 달팽이, 오렌지
+- 주제B: 악보, 줄자, 스카치테이프, 자물쇠, 반코팅장갑, 저울, 얼음
+- 조건: 제공된 사물과 이미지 이외의 형상은 표현하지 마시오. 제공된 사물은 모두 1회 이상 표현하시오. 제공된 사물의 색상은 변경하지 마시오.
+- 화지크기 : 켄트지 3절
+- 시험시간 : 5시간
+2.사고의 전환
+- 준비물: 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구
+- 실기주제 : 주제A, 주제B에서 각 1개씩 선정하여 연결된 주제를 당일 추첨 (예시: 콜라병과 계절)
+- 주제A: 콜라병, 포카리스웨트(캔), 마스크, 시계, 맥가이버 칼
+- 주제B: 바이러스, 자유, 여행, 계절, 꿈
+- 화지크기: 켄트지 2절
+- 시험시간: 5시간
+이와 같은 정보는 디자인조형학과 실기시험을 준비하는 데 중요한 요소들입니다. 추가적인 정보나 문의사항이 있다면 "https://ipsi.deu.ac.kr/main.do"를 방문하시기 바랍니다.</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>디자인조형학과의 실기시험은 시각디자인, 산업디자인, 공예디자인 세 가지 종목 중 하나를 선택하여 응시하게 됩니다. 각 종목별로 배점이 다르며, 전체 실기시험 점수는 700점으로 구성됩니다.
+### 디자인조형학과 실기시험 종목별 정보
+#### 1. 시각디자인
+- **배점**: 490점 (70%)
+- **준비물**: 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구
+- **실기주제**: 주제A와 주제B에서 각각 하나를 선택하여 연결된 주제로 작업합니다. 예시로는 "잠자리와 저울" 또는 "콜라병과 계절"과 같은 주제가 될 수 있습니다.
+- **화지크기**: 켄트지 3절
+- **시간**: 5시간
+#### 2. 산업디자인
+- **배점**: 140점 (20%)
+- **준비물**: 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구
+- **실기주제**: 주제A와 주제B에서 각각 하나를 선택하여 연결된 주제로 작업합니다. 예시로는 "콜라병과 계절" 또는 "잠자리와 저울"과 같은 주제가 될 수 있습니다.
+- **화지크기**: 켄트지 2절
+- **시간**: 5시간
+#### 3. 공예디자인
+- **배점**: 70점 (10%)
+- **준비물**: 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구
+- **실기주제**: 주제A와 주제B에서 각각 하나를 선택하여 연결된 주제로 작업합니다. 예시로는 "콜라병과 계절" 또는 "잠자리와 저울"과 같은 주제가 될 수 있습니다.
+- **화지크기**: 켄트지 2절
+- **시간**: 5시간
+### 준비사항 및 주의사항
+1. **준비물**: 모든 종목에서 볼펜, 연필, 색연필, 수채물감 등이 필요합니다. 개인적으로 필요한 도구를 가져와야 합니다.
+2. **주제 선정**: 당일에 주어지는 주제 중에서 각각 하나씩 선택하여 작업해야 합니다.
+3. **화지크기 및 시간**: 모든 종목은 켄트지 3절 또는 2절을 사용하며, 작업 시간은 5시간입니다.
+### 추가 정보
+- **주제 선정 방법**: 당일에 추첨을 통해 주제가 결정됩니다.
+- **표현 제한**: 제공된 사물과 이미지는 표현할 수 있지만, 다른 형상은 표현하지 않아야 합니다. 또한 색상 변경도 금지되어 있습니다.
+이러한 정보를 참고하여 디자인조형학과의 실기시험을 준비하시면 도움이 될 것입니다.</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>0.3280925695162146</v>
+        <v>0.383006552518799</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Google Gemma-2-9b-it Average</t>
+          <t>Qwen2.5-7B-instruct</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>디자인조형학과의 실기종목, 준비물, 실기주제, 화지크기, 시간에 대한 정보는 다음과 같습니다:
+1.실기종목: 기초디자인
+- 준비물: 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구
+- 실기주제: 주제A, 주제B에서 각 1개씩 선정하여 연결된 주제를 당일 추첨 (예시: 잠자리와 저울)
+- 주제A: 잠자리, 무궁화, 피망, 고양이, 양파, 달팽이, 오렌지
+- 주제B: 악보, 줄자, 스카치테이프, 자물쇠, 반코팅장갑, 저울, 얼음
+- 조건: 제공된 사물과 이미지 이외의 형상은 표현하지 마시오. 제공된 사물은 모두 1회 이상 표현하시오. 제공된 사물의 색상은 변경하지 마시오.
+- 화지크기: 켄트지 3절
+- 시간: 5시간
+2.실기종목: 사고의 전환
+- 준비물: 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구
+- 실기주제: 주제A, 주제B에서 각 1개씩 선정하여 연결된 주제를 당일 추첨 (예시: 콜라병과 계절)
+- 주제A: 콜라병, 포카리스웨트(캔), 마스크, 시계, 맥가이버 칼
+- 주제B: 바이러스, 자유, 여행, 계절, 꿈
+- 화지크기: 켄트지 2절
+- 시간: 5시간</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>디자인조형학과의 실기종목은 다음과 같습니다:
+- **시각디자인**
+- **산업디자인**
+- **공예디자인**
+- **기초디자인 / 사고의 전환**
+각 종목별 배점 비율은 다음과 같습니다:
+- 시각디자인: 70%
+- 산업디자인: 30%
+**준비물**: 볼펜, 연필, 색연필, 수채물감 등 표현에 필요한 도구가 필요합니다.
+**실기주제**: 주제A와 주제B에서 각각 1개씩 선정하여 연결된 주제를 당일 추첨으로 결정합니다. 예시로는 다음과 같은 주제들이 있습니다:
+- **기초디자인 / 사고의 전환**
+  - 주제A: 잠자리, 무궁화, 피망, 고양이, 양파, 달팽이, 오렌지
+  - 주제B: 악보, 줄자, 스카치테이프, 자물쇠, 반코팅장갑, 저울, 얼음
+**화지크기**: 켄트지3절 또는 켄트지2절 (종류에 따라 다름)
+**시간**: 5시간
+위 정보는 각 실기 종목별로 동일하게 적용됩니다.</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>0.2682980797791024</v>
+        <v>0.4882511112590651</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Meta Llama-3.1-Instruct Average</t>
+          <t>Qwen2.5-7B-instruct</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>경기지도학과 모집종목별 인정대회는 다음과 같습니다:
+배드민턴(남)
+- 한국중·고연맹회장기전국학생선수권대회
+- 대한배드민턴협회장기전국종별배드민턴선수권대회
+- 전국학교대항배드민턴선수권대회
+- 전국종별배드민턴선수권대회
+- 전국연맹종별배드민턴선수권대회
+- 전국체육대회
+- 각종국제대회
+- 주니어국제대회(국가대표팀, 주니어팀 소속으로 출전한 대회만 인정)
+- 광역시·도 협회장기 종별대회
+축구(남)
+- 춘계한국고등학교축구연맹전
+- 추계한국고등학교축구연맹전
+- 대한축구협회장배전국고등학교축구대회
+- 문화체육관광부장관기전국고등학교축구대회
+- 문화체육관광부장관배전국고등학교축구대회
+- 백운기전국고등학교축구대회
+- 전국고등축구리그(권역별고교축구리그)
+- 전국고등축구리그왕중왕전
+- 무학기전국고등학교축구대회
+- 청룡기전국고등학교축구대회
+- 백록기전국고등학교축구대회
+- 금강대기전국고등학교축구대회
+- 대통령금배전국고등학교축구대회
+- 금석배전국고등학생축구대회
+- 부산MBC전국고등학생축구대회
+- K리그 U18 챔피언십
+- K리그 U18 챔피언십왕중왕전</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t xml:space="preserve"> 경기지도학과 모집종목별 인정대회에 다음과 같은 대회들이 포함됩니다:
+배드민턴(남):
+- 한국중·고연맹회장기 전국학생선수권대회
+- 대한배드민턴협회장기 전국종별배드민턴선수권대회 
+- 전국학교대항배드민턴선수권대회
+- 전국종별배드민턴선수권대회
+- 전국연맹종별배드민턴선수권대회
+- 전국체육대회
+- 각종 국제대회 (국가대표팀, 주니어팀 소속으로 출전한 대회만 인정)
+- 광역시·도 협회장기 종별대회
+축구(남):
+- 춘계 한국고등학교축구연맹전
+- 추계 한국고등학교축구연맹전
+- 대한축구협회장배 전국고등학교축구대회
+- 문화체육관광부장관기 전국고등학교축구대회
+- 문화체육관광부장관배 전국고등학교축구대회
+- 백운기 전국고등학교축구대회
+- 전국 고등축구리그 (권역별고교축구리그)
+- 전국 고등축구리그 왕중왕전
+- 무학기 전국고등학교축구대회
+- 청룡기 전국고등학교축구대회
+- 백록기 전국고등학교축구대회
+- 금강대기 전국고등학교축구대회
+- 대통령금배 전국고등학교축구대회
+- 금석배 전국고등학생축구대회
+- 부산 MBC 전국고등학생축구대회
+- K리그 U18 챔피언십
+- K리그 U18 챔피언십 왕중왕전</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>0.09430187624113912</v>
+        <v>0.9578833781036659</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>디자인조형학과의 기초디자인 실기시험 주제는 다음과 같습니다:
+- 주제A: 잠자리, 무궁화, 피망, 고양이, 양파, 달팽이, 오렌지
+- 주제B: 악보, 줄자, 스카치테이프, 자물쇠, 반코팅장갑, 저울, 얼음
+시험 당일에는 주제A와 주제B에서 각각 1개씩 선정하여 연결된 주제를 추첨하게 됩니다. 예시로는 "잠자리와 저울"이 있습니다.</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 디자인조형학과의 기초디자인 실기시험에서는 주제A와 주제B를 각각 하나씩 선택하여 연결된 주제로 만듭니다. 제공된 주제들은 다음과 같습니다:
+1. 주제A: 잠자리, 무궁화, 피망, 고양이, 양파, 달팽이, 오렌지
+2. 주제B: 악보, 줄자, 스카치테이프, 자물쇠, 반코팅장갑, 저울, 얼음
+당일에는 이 주제들 중에서 각각 하나씩을 선택하여 연결된 주제를 만듭니다.</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>0.7159861694275004</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>아니요. 학생부 교과 전형에서는 출결 점수가 반영되지 않습니다.</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>2024학년도 동점자 처리기준 표에 따르면, 학생부종합(조기취업형계약학과전형)에서는 교과 성적을 평균하는 방법으로 등급 평균을 산출하는데, 출결 점수가 포함되지 않습니다. 
+따라서, 학생부교과 전형에서 출결 점수는 반영되지 않는 것으로 보입니다.
+만약 다른 전형 유형이나 특정 단과대학의 경우가 다르다면, 해당 정보를 확인하기 위해 공식 홈페이지나 연락처를 통해 문의하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>0.003641548695529096</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>인문사회과학대학의 국어국문학과에서 가군 일반학생 전형으로 17명을 모집합니다.</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>17명을 모집합니다. 
+참조 정보:
+- 표 제목 : 가군 수능(일반학생전형), 실기/실적(일반학생전형) 모집단위 및 모집인원
+- 해당 내용 : 인문사회과학대학 / 인문사회 / 국어국문학과 - 교직 / 17 /
+따라서, 인문사회과학대학의 국어국문학과에서 가군 일반학생 전형으로는 17명을 모집합니다.</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>0.05906330415030002</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 인문사회과학대학 영어영문학과의 경우, 다군 일반학생 전형을 통해 총 28명의 신입생을 선발합니다.</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>28명을 모집합니다.
+인문사회과학대학 / 인문사회 / 영어영문학과 - 교직 / 28 /
+이 항목은 다군 수능(일반학생전형)의 모집단위와 모집인원을 나타내고 있으며, 영어영문학과 - 교직의 경우 28명을 모집한다고 명시되어 있습니다.</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>0.152471578544296</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 의료보건생활대학 간호학과의 경우, 나군 일반학생 전형을 통해 총 22명의 신입생을 선발합니다.</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 의료보건생활대학 간호학과의 나군 일반학생전형 모집인원은 110명입니다.</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>0.533334865391997</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>수능 영어영역 등급에 따른 점수는 다음과 같습니다:
+- 1등급: 139점
+- 2등급: 131점
+- 3등급: 123점
+- 4등급: 115점
+- 5등급: 107점
+- 6등급: 99점
+- 7등급: 91점
+- 8등급: 83점
+- 9등급: 75점</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 수능 영어 등급에 따른 점수는 다음과 같습니다:
+1등급: 139  
+2등급: 131  
+3등급: 123  
+4등급: 115  
+5등급: 107  
+6등급: 99  
+7등급: 91  
+8등급: 83  
+9등급: 75  
+이 점수들은 각 등급에 해당하는 수능 영어 성적을 받은 학생들이 받는 평균 점수입니다.</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>0.680574452218573</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>아니요, 예술고 학생은 나군 학생부교과 농어촌학생전형으로 지원할 수 없습니다. 지원자격에 따르면 농어촌지역 또는 도서·벽지에 소재한 특수목적고 중 과학고, 국제고, 외국어고, 체육고, 예술고 출신자는 지원할 수 없습니다.</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 예술고 학생은 나군 학생부교과(농어촌학생전형)로 지원할 수 없습니다. 
+표에서 확인할 수 있는 내용에 따르면, 특성화고의 경우 다음과 같이 제한되어 있습니다:
+- 특성화고 { 특성(직업) / 특성(대안) }
+  - 지원 가능
+  - 지원 가능
+  - 지원 가능
+  - 지원 가능
+  - 지원 불가능 
+  - 지원 불가능
+특히 예술고는 "지원 불가능"으로 표기되어 있어, 예술고 학생은 나군 학생부교과(농어촌학생전형)로 지원할 수 없습니다.
+따라서 예술고 학생이 농어촌 지역에서 교육받았다면 다른 특성화고나 일반 고등학교를 통해 이 전형을 신청해야 합니다.</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>0.1394864822576465</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>레저스포츠학과 여자 제자리 멀리뛰기 4등급 기록과 배점은 다음과 같습니다:
+- 기록: 218~221 cm
+- 배점: 275점</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>4등급의 제자리 멀리뛰기 여자 기록은 252~255cm이며, 이 기록에 대한 배점은 175점입니다.
+따라서 레저스포츠학과 여자 4등급 제자리 멀리뛰기는 252~255cm를 달성하면 175점을 받을 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>0.283676934858839</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>경기지도학과의 출결 반영 비율은 12%입니다.</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 경기지도학과 실기/실적(경기실적우수자전형)에서는 출결이 12%를 반영합니다.
+상세 정보는 다음과 같습니다:
+- 학생부 교과성적 : 18%
+- 출결 : 12%
+- 서류(경기실적) : 70%
+따라서 경기지도학과의 경우, 출결은 총 전형요소 중에서 12%를 차지합니다.</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>0.002014742786565004</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>동의대학교 2024학년도 가군에서 물리치료학과는 4명을 모집합니다.</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 가군에서 물리치료학과는 3명을 모집합니다.</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>0.8886038899541627</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>2024. 01. 17.(수) 입니다.</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>2024학년도 나군 실기/실적 전형에서 디자인조형학과의 실기고사는 1월 17일(수)에 실시됩니다.
+관련 정보는 다음과 같습니다:
+- **일정**: 2024. 01. 17.(수)
+- **대기실 및 입실시간 안내**: 2024. 01. 12.(금) 14:00 이후, 입학안내 홈페이지에서 조회 가능
+이 정보는 [전형일정] 표에서 확인할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>0.0002554384453990063</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>수능 최저 학력 기준은 없습니다.</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 응용화학과의 정확한 수능 최저기준 정보가 제공된 표에서 확인할 수 없습니다. 제공된 표는 각 전형 유형별로 수능 최저기준이 없음을 나타내고 있으며, 응용화학과는 특정 전형 유형에 속하지 않습니다.
+만약 응용화학과의 수능 최저기준을 알고 싶다면, 다음과 같은 방법을 추천드립니다:
+1. 동의대학교 입학처 웹사이트를 방문하여 공식 안내서나 주요 변경사항을 확인합니다.
+2. 입학사정관이 참여하는 전형인 경우, 해당 전형의 특별한 수능 최저기준이 정해져 있을 수 있습니다.
+3. 직접 동의대학교 입학처에 문의하여 가장 정확한 정보를 얻는 것이 좋습니다.
+현재 제공된 표에서는 응용화학과의 수능 최저기준을 확인할 수 없습니다. 추가 정보가 필요하다면 위 방법들을 활용해보세요.</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>1.431185283090417e-10</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>동의대학교 2024학년도에 신설된 학과는 다음과 같습니다:
+1. 심리학과
+2. 스마트항만물류학과
+3. 창업투자경영학과
+4. 라이프융합학부 (스타트업창업투자학, 뷰티비즈니스학, 라이프생활문화학)
+5. 경기지도학과</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교에서 신설된 학과로는 다음과 같습니다:
+1. 경기지도학과 (신설)
+2. 라이프융합학부 (신설) - 스타트업창업투자학, 뷰티비즈니스학, 라이프생활문화학 포함
+3. 부동산자산경역학부 (신설) - 부동산투자학, 부동산개발경영학 포함
+위와 같이 동의대학교에서는 2024학년도에 세 가지 신설 학과를 도입하였습니다.</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>0.4882314073816491</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>동의대학교 2024학년도 나군의 학생부종합(성인학습자전형)의 전형요소 반영비율은 서류 70%, 면접 30%입니다.</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 나군의 학생부종합(성인학습자전형)의 전형요소 반영비율은 다음과 같습니다:
+- 서류 평가: 70%
+- 면접 평가: 30%
+이 비율은 성인학습자전형에 적용되는 일반적인 규칙이며, 다른 학생부종합 전형과 동일합니다.</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>0.2964669790655702</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>동의대학교에서는 다음 모집단위에서 수능 가산점을 적용합니다:
+- 의료·보건·생활대학
+- 공과대학
+- ICT융합공과대학
+이들 모집단위에서 수학(미적분 또는 기하)을 응시한 경우, 수학 취득 표준점수의 10%를 가산점으로 부여합니다.</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 동의대학교에서는 의료·보건·생활대학, 공과대학, ICT융합공과대학 모집단위에서 수능 수학(미적분 또는 기하) 응시자에게 가산점이 부여됩니다. 이 경우 수학 취득 표준점수의 10%가 추가 점수가 됩니다.
+따라서, 해당 학과에서 수학을 응시한 학생들은 그 점수가 10% 증가하여 총 성적에 반영됩니다.</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>0.5512899792741847</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>동의대학교의 2024학년도 가군 수능(일반학생전형)에서는 수능 성적을 100% 반영합니다. 자세한 수능 성적 반영 방법은 '38페이지 Ⅴ. 수능성적 반영방법'을 참조하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 가군에서는 수능 성적이 전 모집단위에 대해 100%로 반영됩니다.
+이 정보는 "다군 수능(일반학생전형) 전형요소 반영비율" 표에서 확인할 수 있으며, 해당 표에는 다음과 같이 명시되어 있습니다:
+```
+다군 수능(일반학생전형) / 전 모집단위 / { 100% / } /
+```
+따라서 가군의 모든 모집단위는 지원자의 수능 성적을 100%로 반영합니다.</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>0.1927561399264988</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>동의대학교 2024학년도 가군 실기고사는 2024년 1월 16일(화)에 진행됩니다.</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 가군 실기고사는 레저스포츠학과와 태권도학과에서 실시되며, 날짜는 2024년 1월 16일(화)입니다.</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>0.4881459582059889</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>동의대학교 2024학년도 나군 수능(일반학생전형) 전형에서는 한의예과, 디자인조형학과와 체육학과, 경기지도학과가 제외됩니다.</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 나군 수능(일반학생전형)에서는 한의예과, 디자인조형학과, 체육학과, 경기지도학과가 실기/실적 위주 전형으로 분류되어 제외되었습니다.
+이 점을 고려하여 나군 수능(일반학생전형)은 전 모집단위에서 한의예과(수학(미적분/기하), 수학(확률과통계))만 제외된 상태로 진행됩니다.</t>
+        </is>
+      </c>
+      <c r="D290" t="n">
+        <v>0.2132588354333095</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2024학년도 동의대의 다군 전형에서는 수능 최저기준이 적용되지 않습니다. </t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교의 다군 전형에서 수능 최저기준은 적용되지 않습니다. 이는 표에서 "수능최저기준 없음"으로 명시되어 있습니다.
+관련 정보:
+- [표 제목] : 다군 수능(일반학생전형) 전형요소 반영비율
+- [표 내용] :
+```
+다군 수능(일반학생전형) / 180 / 일괄 합산 / { 0 /  0 /  0 /  0 /  0 /  100 / } / 수능최저기준 없음 /
+```
+따라서, 다군 전형에서는 수능 최저기준이 적용되지 않습니다.</t>
+        </is>
+      </c>
+      <c r="D291" t="n">
+        <v>0.006022310933337018</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대에서 학부에서 학과로 분리된 학과는 다음과 같습니다:
+1. 보육가정상담학과 → 아동학과
+2. 경제금융보험학과 → 금융경영학과
+3. 정보경영학부 → 경영정보학과, e비즈니스학과
+4. 부동산금융자산경영학과 → 부동산자산경영학부(부동산투자학, 부동산개발경영학)
+5. 기계자동차로봇부품공학부 → 기계공학과, 로봇자동화공학과, 자동차공학과
+6. 신소재공학부(금속소재공학, 전기전자소재공학, 고분자소재공학) → 신소재공학과, 고분자나노공학과
+7. 건설공학부(건축학(5년제), 건축공학, 토목공학, 도시공학) → 건축학과(5년제), 건축공학과, 토목공학과, 도시공학과
+8. 화학환경공학부(화학공학, 환경공학, 응용화학) → 화학공학과, 환경공학과, 응용화학과
+9. 바이오응용공학부(의생명공학, 바이오의약공학, 식품공학) → 의생명공학과, 바이오의약공학과, 식품공학과
+10. 디자인공학부(인간시스템디자인공학, 제품디자인공학) → 인간공학과, 제품디자인공학과
+11. 산업융합시스템공학부(산업ICT기술공학, 산업경영빅데이터공학) → 산업경영빅데이터공학과
+12. 창의소프트웨어공학부(컴퓨터소프트웨어공학, 응용소프트웨어공학) → 소프트웨어공학부(컴퓨터소프트웨어공학, 응용소프트웨어공학)
+13. 전기전자통신공학부(전기공학, 전자공학, 정보통신공학) → 전기공학과, 전자공학과
+14. 음악학과(성악, 피아노, 관현타악, 실용음악뮤지컬, 뉴미디어작곡) → 음악학과(클래식, 실용음악, 뉴미디어작곡)</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교에서는 여러 학과가 학부에서 학과로 분리되었습니다. 특히 다음과 같은 학과들이 학부에서 학과로 분리되었습니다:
+1. 보육·가정상담학과 - 아동학과
+2. 경제금융보험학과 - 금융경영학과
+3. 정보경영학부(경영정보학, e비즈니스학) - 경영정보학과, e비즈니스학과
+4. 부동산금융·자산경영학과 - 부동산투자학, 부동산개발경영학
+5. 기계자동차로봇부품공학부(기계공학, 로봇·자동화공학, 자동차공학) - 기계공학과, 로봇자동화공학과, 자동차공학과
+6. 신소재공학부(금속소재공학, 전기전자소재공학, 고분자소재공학) - 신소재공학과, 고분자나노공학과
+7. 건설공학부(건축학(5년제), 건축공학, 토목공학, 도시공학) - 건축학과(5년제), 건축공학과, 토목공학과, 도시공학과
+8. 화학환경공학부(화학공학, 환경공학, 응용화학) - 화학공학과, 환경공학과, 응용화학과
+9. 바이오응용공학부(의생명공학, 바이오의약공학, 식품공학) - 의생명공학과, 바이오의약공학과, 식품공학과
+10. 디자인공학부(인간·시스템디자인공학, 제품디자인공학) - 인간공학과, 제품디자인공학과
+11. 산업융합시스템공학부(산업ICT기술공학, 산업경영빅데이터공학) - 산업경영빅데이터공학과
+이 외에도 일부 학과는 학부 통합 또는 명칭 변경을 통해 변화하였습니다.</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>0.7346522753753296</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>동의대학교 2024학년도 전형일정에서 원서접수 마감일은 2024년 1월 6일(토) 18시입니다.</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 전형일정에 따르면, 원서접수 마감일은 **2024. 01. 06.(토) 18시**까지입니다.
+추가 유의사항:
+- 원서접수 사이트 접속이 마감일 정각에 차단되므로 사전에 미리 접속하여 지원 내용 입력 및 전형료 결제를 완료해야 합니다.
+- 마감 시한까지 원서접수를 완료하지 못한 경우 지원자 본인의 책임이므로 유의하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>0.04703830493623421</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t xml:space="preserve">동의대 2024학년도에 전형 요소 변화가 있는 전형은 다음과 같습니다:
+1.  학생부종합(성인학습자전형):
+ - 2023학년도: 특성화고 등을 졸업한 재직자
+ - 2024학년도: 고교 졸업(예정)자 또는 법령에 의한 동등 학력 소지자로서 만 30세 이상인 자
+2.  학생부종합(조기취업형계약학과전형):
+  - 2023학년도: 서류(학생부) 70% + 면접 30%
+  - 2024학년도: 서류(학생부) 60% + 면접 40%
+3. 실기/실적(경기실적우수자전형):
+  - 2023학년도: 학생부교과(출결 포함) 30% + 서류(실적) 70%
+  - 2024학년도: 학생부교과 18% + 출결 12% + 서류(실적) 70%
+4. 반영학기(학생부교과, 실기/실적 위주전형):
+ - 2023학년도: 
+  - 고교 졸업예정자 : 1학년 1학기~3학년 1학기
+  - 고교 졸업자 : 1학년 1학기~3학년 2학기
+ - 2024학년도: 
+  -고교 졸업(예정)자 : 1학년 1학기~3학년 1학기
+5. 반영과목(학생부교과, 실기/실적 위주전형):
+ - 2023학년도:
+  -전 모집단위(한의예과 제외):
+   -국어, 수학, 영어교과 중 석차등급 상위 8과목
+   -8과목을 제외한 국어, 수학, 영어, 한국사, 사회(역사/도덕 포함), 과학교과 중 석차등급 상위 4과목
+   -반영교과 중 진로선택과목 최대 2개 이내 반영 가능
+   -진로선택과목 성적반영: A: 2등급, B: 4등급, C: 6등급
+  -한의예과:
+   -국어, 수학, 영어, 한국사, 사회(역사/도덕 포함), 과학, 한문교과 전과목
+   -진로선택과목: 미반영
+- 2024학년도:
+  -전 모집단위(한의예과 제외):
+   -국어, 수학, 영어, 한국사, 사회(역사/도덕 포함), 과학교과 중 석차등급 상위 12과목
+   -반영교과 중 진로선택과목 최대 2개 이내 반영 가능
+   -진로선택과목 성적반영: A: 1등급, B: 3등급, C: 5등급
+  -한의예과:
+   -국어, 수학, 영어, 한국사, 사회(역사/도덕 포함), 과학, 한문교과 전과목
+   -진로선택과목: 반영교과 전과목 반영
+</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교에서 주요 전형 요소 변화는 다음과 같습니다:
+1. **가군 수능(일반학생전형)**
+   - 전형 요소 반영 비율이 변경되지 않았습니다.
+   - 수능 최저기준은 없습니다.
+2. **나군 실기/실적(일반학생전형)**
+   - 레저스포츠학과와 태권도학과는 실기 70%, 수능 30%로 변경되었습니다.
+   - 디자인조형학과와 체육학과는 실기 70%, 수능 30%로 변경되었습니다.
+3. **나군 학생부교과(농어촌학생전형)**
+   - 전형 요소 반영 비율이 100%로 변경되었습니다.
+   - 수능 최저기준은 없습니다.
+4. **나군 학생부교과(평생학습자전형)**
+   - 서류가 70%, 수능이 30%로 변경되었습니다.
+   - 수능 최저기준은 없습니다.
+5. **나군 학생부교과(성인학습자(정원내)전형)**
+   - 서류가 70%, 수능이 30%로 변경되었습니다.
+   - 수능 최저기준은 없습니다.
+6. **나군 학생부종합(재직자전형)**
+   - 서류가 70%, 수능이 30%로 변경되었습니다.
+   - 수능 최저기준은 없습니다.
+7. **나군 학생부종합(조기취업형계약학과전형)**
+   - 서류가 60%, 수능이 40%로 변경되었습니다.
+   - 수능 최저기준은 없습니다.
+이러한 변화는 전반적으로 실기와 학생부교과, 학생부종합 전형에서 수능의 비중을 줄이고, 서류 및 실기의 비중을 늘리는 방향으로 조정되었습니다.</t>
+        </is>
+      </c>
+      <c r="D294" t="n">
+        <v>0.2803795723874063</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>동의대학교 2024학년도 가군 실기/실적 전형에서 실기 비중은 70%입니다.</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 가군 실기/실적 전형에서 실기 비중은 70%입니다.
+이는 "나군 실기/실적(경기실적우수자전형) 전형요소 반영비율" 표에서 확인할 수 있습니다:
+```
+경기지도학과 / { 18% /  12% /  70% / }
+```
+여기서 70%는 실기 비중을 나타냅니다.</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>0.04738692425475222</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>동의대 2024학년도 신설된 라이프융합학부의 세부 전공은 다음과 같이 구성되어 있습니다:
+ - 스타트업창업투자학
+ - 뷰티비즈니스학
+ - 라이프생활문화학</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>2024학년도 동국대학교에서 신설된 '라이프융합학부'는 세부 전공으로 다음과 같이 구성되어 있습니다:
+- 스타트업 창업투자학
+- 뷰티 비즈니스학  
+- 라이프 생활문화학
+这三个专业方向共同构成了生活融合学部的新设课程。</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>0.6224004329549351</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>동의대 2024학년도 가군에서 실기고사에 참여해야 하는 학과는 다음과 같습니다:
+1. 체육학과
+2. 레저스포츠학과</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 가군에서 실기고사에 참여해야 하는 학과는 다음과 같습니다:
+1. 레저스포츠학과 (태권도 포함)
+2. 디자인조형학과 (시각디자인, 산업디자인, 공예디자인)
+3. 체육학과
+이러한 학과들은 가군 수능(일반학생전형)에서 실기고사를 진행합니다.</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>0.249650172574482</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">동의대 2024학년도 실기/실적 위주 전형 지원 가능한 학과는 다음과 같습니다:
+1. 레저스포츠학과
+2. 태권도학과
+3. 디자인조형학과
+4. 체육학과
+5. 경기지도학과 </t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교에서 실기/실적 위주 전형인 "가군 실기/실적(일반학생전형)"과 "나군 실기/실적(일반학생전형)"에 지원할 수 있는 학과는 다음과 같습니다:
+1. 가군 실기/실적(일반학생전형):
+   - 레저스포츠학과
+   - 태권도학과
+2. 나군 실기/실적(일반학생전형):
+   - 디자인조형학과 (시각디자인, 산업디자인, 공예디자인)
+   - 체육학과
+이러한 학과들은 해당 전형의 특성상 실기나 실적을 평가하는 요소를 포함하고 있습니다. 지원하려는 학과가 이 목록에 포함되어 있다면, 실기/실적 위주 전형을 지원할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>0.08986439299150421</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>동의대학교의 라이프융합학부는 신설된 학부로, 다음과 같은 전공을 제공합니다:
+ - 스타트업창업투자학
+ - 뷰티비즈니스학
+ - 라이프생활문화학</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 동의대학교 미래융합대학의 라이프융합학부는 신설된 학부로, 다음과 같은 전공들을 포함하고 있습니다:
+- 스타트업창업투자학
+- 뷰티비즈니스학
+- 라이프생활문화학
+这三个专业都是该新设立的学部的一部分。</t>
+        </is>
+      </c>
+      <c r="D299" t="n">
+        <v>0.622532105274743</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>특수목적고등학교 출신 학생은 일반학생전형으로 지원할 수 있습니다. 다만, 농어촌학생전형의 경우 마이스터고를 제외한 특수목적고등학교 출신자는 지원할 수 없습니다. 일반학생전형에 대한 자세한 정보는 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>你在询问是否可以作为特殊教育高中学生申请동의大学的一般学生入学考试。根据提供的信息，东义大学的普通学生招生中，并没有明确排除特殊教育高中的毕业生。
+但是，为了确保你的资格，请参考以下几点：
+1. **招生对象**：一般学生入学通常面向普通高中毕业生或同等学历者开放。
+2. **特殊教育高中**：虽然没有直接说明，但如果你是特殊教育高中毕业且具备相应的学业能力，你可能仍然有资格申请。建议查看东义大学的具体招生简章或联系学校确认。
+你可以访问东义大学的官方网站（https://ipsi.deu.ac.kr/main.do），在“招生信息”部分查找更详细的信息，或者直接咨询学校的招生办公室以获得最准确的答案。
+希望这些信息对你有所帮助！如果有其他问题，请随时提问。</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>0.07718200961405976</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대 나군 전형에서 가장 많이 모집하는 학과는 인문사회과학대학의 중어중국학과와 공과대학 신소재공학과로, 나군 일반학생 전형에서 32명을 모집합니다.</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>2024학년도 동의대학교 나군 전형에서 가장 많이 모집하는 학과를 파악하기 위해서는 각 학과별로 정원을 확인해야 합니다. 제공된 표 중에서 나군 학생부종합(평생학습자전형, 성인학습자전형, 재직자전형) - 정원외 모집단위 및 모집인원에 대한 정보를 보면:
+- 스마트호스피탈리티학과: 7명
+- 미래형자동차학과: 7명
+- 소프트웨어융합학과: 7명
+이 세 학과 모두 같은 정원인 7명을 모집하고 있습니다. 그러나 나군 전형의 전체적인 모집 인원을 고려해야 합니다.
+다른 나군 전형에서의 정원을 확인해보면:
+- 학생부교과(농어촌학생전형) - 정원외: 16명
+- 학생부종합(재직자전형) - 정원외: 7명 (두 개 모두)
+- 학생부종합(조기취업형계약학과전형) - 정원외: 21명
+이 중에서 가장 많은 모집 인원을 보이는 학과는 **학생부교과(농어촌학생전형) - 정원외**로, 16명을 모집하고 있습니다.
+따라서, 2024학년도 동의대학교 나군 전형에서 가장 많이 모집하는 학과는 **학생부교과(농어촌학생전형) - 정원외** 학과입니다.</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>0.003718874195271592</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>마이스터고를 제외한 특수목적고등학교 출신자는 동의대 학생부교과 농어촌학생전형으로 지원할 수 없습니다.  지원 자격에 따르면, 농어촌지역 또는 도서·벽지에 소재한 특수목적고 중 과학고, 국제고, 외국어고, 체육고, 예술고 출신자는 지원할 수 없습니다.</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>你是中国人，所以这里我将回答转换成了中文。
+是的，你可以申请东义大学的学生部教科农渔村学生类型。根据提供的信息，特殊目的高中毕业生符合农渔村学生的资格条件之一：
+1. 在农村（镇、乡）地区中学完成整个教育过程，并且在中学学习期间（初中入学日~高中毕业日），本人及其父母双方（如果父母一方去世或离婚，则不包括该方）均居住在农村（镇、乡）地区。居住地和学生的学校可以不同。
+2. 无需考虑父母的居住地，只要你在整个初、中、高教育过程中，在农渔村（镇、乡）地区的学校完成并居住即可。
+为了申请，请确保准备以下文件：
+1. 本人及其父母双方的户籍证明书各一份。
+2. 中学和高中期间的学生生活记录表各一份。
+3. 如果父母一方去世，需要提供死亡证明书；如果父母离婚，则需提供监护权证明书及本人的基本信息证明书。
+提交期限为2024年1月3日至1月12日（周五）17:00前。请将文件邮寄至：47340 韩国釜山市东区엄광路176号 东义大学招生办公室。
+请注意，如果最终注册者是高中毕业生，则需要在2024年2月16日（周五）之前提交毕业证明书。</t>
+        </is>
+      </c>
+      <c r="D302" t="n">
+        <v>1.190491134552565e-79</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>제공된 정시 모집요강에는 2024학년도 소프트웨어공학부 합격자 평균 성적에 대한 정보가 포함되어 있지 않습니다. 해당 정보를 확인하려면 "https://ipsi.deu.ac.kr/main.do"를 방문하여 문의하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 제공된 정보로는 2024학년도 소프트웨어공학부의 합격자 평균 성적이 직접적으로 나와 있지 않습니다. 
+가능한 해결 방법은 다음과 같습니다:
+1. **수능(일반학생전형) 최종등록자 표**를 확인해 보세요: 이 표에는 각 모집단위별로 합격자의 평균 성적과 관련 정보가 포함되어 있을 수 있습니다.
+2. **나군 학생부종합 전형의 서류평가 영역 및 배점 표**를 참조하세요: 이 표에서는 학업역량과 전공적합성 등 평가 항목별로 점수 배점을 볼 수 있지만, 실제 합격자들의 성적이 포함되어 있지 않을 것입니다.
+3. **입학관리팀에 문의해 보세요**: 직접적인 정보를 얻기 위해서는 입학관리팀이나 관련 부서에 문의하는 것이 가장 정확한 방법입니다.
+4. **전형일정 표**를 확인하세요: 이 표에는 합격자 발표와 등록 일정이 포함되어 있지만, 성적 정보는 없습니다.
+추가적인 정보나 자세한 질문이 있으시다면 언제든지 알려주세요!</t>
+        </is>
+      </c>
+      <c r="D303" t="n">
+        <v>0.02918772833504308</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>제공된 정시 모집요강에는 2024학년도 소프트웨어공학부 합격자 평균 성적에 대한 정보가 포함되어 있지 않습니다. 해당 정보를 확인하려면 "https://ipsi.deu.ac.kr/main.do"를 방문하여 문의하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 제공된 정보로는 2024학년도 소프트웨어공학부 최초합격자의 평균성적이 포함되어 있지 않습니다. 
+현재 데이터에서는 수능(일반학생전형)의 최초합격자와 최종등록자의 성적 통계가 일부 제공되고 있지만, 특정 학과별로 구체적인 성적 정보는 없습니다.
+만약 소프트웨어공학부의 최초합격자 평균성적을 알고 싶다면, 다음과 같은 방법이 있습니다:
+1. 동의대학교 입학관리 홈페이지를 확인해 보세요.
+2. 해당 학과의 공지사항이나 통계 정보를 찾아보세요.
+3. 입학처에 직접 문의하여 요청하시면 더 정확한 정보를 얻을 수 있습니다.
+추가적으로, 제공된 표에서는 다른 학과들의 최초합격자와 최종등록자의 성적 통계만 포함되어 있으므로, 특정 학과의 성적 정보는 추가적인 자료 검색이 필요할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D304" t="n">
+        <v>0.05701672778841026</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>합격자 발표 일정은 다음과 같습니다:
+ - 최초 합격자 발표: 2024년 2월 2일(금) 14:00
+ - 충원 합격자 1차 발표: 2024년 2월 14일(수) 09:00
+ - 충원 합격자 2차 발표: 2024년 2월 15일(목) 09:00
+ - 충원 합격자 3차 이후 발표: 2024년 2월 15일(목) 19:00부터 2024년 2월 20일(화) 18:00까지
+ 모든 발표는 홈페이지를 통해 개별 조회해야 합니다.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>2024년 나군의 합격자 발표 일정에 대한 정보는 다음과 같습니다:
+- 최초합격자는 홈페이지를 통해 실시됩니다.
+- 1차, 2차 충원합격자는 발표일은 명시되어 있습니다. 
+- 3차 이후 충원합격자는 2024년 2월 15일(목)부터 2024년 2월 20일(화)까지의 기간에 발표됩니다.
+따라서 합격자 발표 일정은 다음과 같습니다:
+- 최초합격자: 홈페이지를 통해 실시
+- 1차 충원합격자: 홈페이지를 통해 실시 (확실한 날짜 미기재)
+- 2차 충원합격자: 홈페이지를 통해 실시 (확실한 날짜 미기재)
+- 3차 이후 충원합격자: 2024년 2월 15일(목)부터 2024년 2월 20일(화)까지
+모든 지원자는 이 기간 내에 합격 여부를 반드시 확인해야 합니다.</t>
+        </is>
+      </c>
+      <c r="D305" t="n">
+        <v>0.366408996013455</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>나군 평생학습자전형, 성인학습자(정원내)전형, 성인학습자(정원외)전형, 재직자전형, 조기취업형계약학과전형의 면접고사 일정은 2024. 01. 20.(토)입니다.</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 면접은 개별적으로 진행되며, 평균적으로 1인당 10분 이내로 이루어집니다. 정확한 시간과 일정은 입학처에서 안내会给您提供的信息显示，面试是个人进行的，每位考生大约需要10分钟以内的时间。具体的面试时间和日期通常由招生办公室通知，请参考相关通知或联系学校以获取确切的日程安排。
+如果您有其他问题或需要进一步的帮助，请告诉我！</t>
+        </is>
+      </c>
+      <c r="D306" t="n">
+        <v>0.06758073659039429</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>동의대 한의예과의 최저학력 기준이 없습니다.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>提供的信息中并没有直接提到韩医系（한의예과）的最低入学资格要求。不过，根据已有的信息可以推测一些可能的要求：
+1. 高中毕业或同等学历是基本要求。
+2. 数学和英语可能会有特定的要求，尤其是对于数学（微积分/几何、概率与统计），因为表格中提到了韩医系在这些科目上有不同的处理方式。
+3. 由于韩医系的特殊性，可能还需要参加一些专门的入学考试或面试。
+4. 可能会有健康相关的要求，因为这是医学专业。
+5. 其他特定的专业要求可能会根据学校的具体规定有所不同。
+要获取最准确的最低学力标准信息，建议直接访问该大学的官方网站（http://ipsi.deu.ac.kr）查看最新的招生简章或联系学校的招生办公室。</t>
+        </is>
+      </c>
+      <c r="D307" t="n">
+        <v>6.331916291663653e-06</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>동의대학교는 수능 최저학력 기준이 없습니다.</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>2024년도 정시모집에서 수능 최저학력 기준은 없습니다. 관련 내용은 다음과 같습니다:
+- 가군 수능(일반학생전형) 전 모집단위(레저스포츠학과, 태권도학과 제외): 수능최저기준 없음
+- 나군 수능(일반학생전형) 전 모집단위(한의예과, 디자인조형학과, 체육학과, 경기지도학과 제외): 수능최저기준 없음 
+- 다군 수능(일반학생전형) 전 모집단위: 수능최저기준 없음
+따라서 정시모집에서는 수능 최저학력 기준이 적용되지 않습니다.</t>
+        </is>
+      </c>
+      <c r="D308" t="n">
+        <v>3.737299336650795e-05</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>충원합격자 발표 일정은 다음과 같습니다:
+ 1. 1차 충원합격자 발표: 2024년 2월 14일(수) 09:00
+ 2. 2차 충원합격자 발표: 2024년 2월 15일(목) 09:00
+ 3. 3차 이후 충원합격자 발표: 2024년 2월 15일(목) 19:00부터 2024년 2월 20일(화) 18시까지</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>2024년 2월 15일(목)부터 3차 이후의 충원합격자를 발표합니다. 구체적으로:
+- 2024년 2월 14일(수) 09:00에 1차 충원 합격자 발표
+- 2024년 2월 15일(목) 09:00에 2차 충원 합격자 발표
+이후 개별 전화 통보 방식으로 추가 충원합격자를 발표하게 됩니다.</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>0.6462962758898457</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>충원합격자 발표 일정은 다음과 같습니다:
+ 1. 1차 충원합격자 발표: 2024년 2월 14일(수) 09:00
+ 2. 2차 충원합격자 발표: 2024년 2월 15일(목) 09:00
+ 3. 3차 이후 충원합격자 발표: 2024년 2월 15일(목) 19:00부터 2024년 2월 20일(화) 18시까지</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>2024년 2월 15일(목)부터 3차 이후 충원합격자를 발표합니다. 이 발표는 개별 전화 통보를 통해 이루어지며, 발표 시간은 2024년 2월 15일(목) 19:00부터 2024년 2월 20일(화) 18시까지입니다.
+발표 후 등록 절차는 개별 전화 통보 시 안내되며, 등록은 지정된 기간 내에 이루어져야 합니다.</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>0.5231194648475864</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>2024년 1월 2일(화) 이후 수시모집 등록자의 등록(입학) 포기로 인한 결원은 정시 일반학생전형 모집인원으로 이월하여 추가로 합격자를 선발합니다. 정시모집 모집단위별 등록인원이 모집인원에 미달된 경우에는 그 인원을 추가모집으로 이월하여 모집합니다.</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>2024년 1월 2일(화) 이후 수시모집 등록자의 등록(입학) 포기로 인한 결원은 정시 일반학생전형 모집인원으로 이월하여 추가로 합격자를 선발합니다. 또한, 모집군별 모집단위별 미등록, 포기 및 환불 등으로 인해 결원이 발생할 경우 그 인원만큼 예비후보 순위에 따라 충원합격자를 선발합니다.
+따라서 추가모집은 가능하며, 정시 일반학생전형 모집인원으로 이월하여 합격자를 선발하거나, 예비후보 순위에 따라 충원합격자를 선발할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>0.4199302942974072</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>평생학습자전형에 대한 정보는 다음과 같습니다.  
+모집단위 및 모집인원
+  - 미래융합대학 라이프융합학부
+  - 전형명: 학생부종합(평생학습자전형)
+  - 모집인원: 11명
+ 지원자격
+ - 평생학습자전형: 고교 졸업(예정)자 또는 법령에 의한 동등학력 소지자
+전형요소 반영 비율
+ - 서류: 70%
+ - 면접: 30%
+ 제출서류
+ - 고교 졸업(예정)자:
+  - 고교 학교생활기록부 1부 (학생부 온라인 제공 동의자는 제출할 필요 없음)
+- 검정고시출신자:
+  - 검정고시 합격증서 사본 또는 합격증명서 1부
+  - 검정고시 성적증명서 1부 (온라인 제공 동의자는 제출할 필요 없음)
+  - 학교생활기록부 대체 서류 (제출여부 선택 가능)
+ - 외국고교 졸업(예정)자:
+  - 공증받은 외국고교 졸업(예정)증명서 1부
+  - 공증받은 외국고교 성적증명서 1부
+  - 학교생활기록부 대체 서류(제출여부 선택 가능)
+  - 외국어로 작성된 경우, 원본과 공증받은 한국어 번역본을 함께 제출
+  - 고교 졸업(예정)증명서, 성적증명서는 해당국가의 정부기관으로부터 아포스티유 확인서 또는 해당국가 주재 한국영사관에서 영사 확인을 발급받아 제출(단, 교육부에서 인정한 재외한국학교는 영사확인 없이 증명서 원본 제출 가능)
+  - 만점이 명시된 고교성적 체계자료를 성적증명서 뒤에 첨부
+  - 최종 등록자 중 외국고교 졸업예정자는 졸업 이후 졸업증명서(아포스티유 확인서 또는 영사확인 
+발급)를 2024. 02. 16.(금)까지 추가 제출하여야 합니다.
+제출기간 및 장소
+ - 제출기간: 2024. 01. 03.(수) ~ 01. 12.(금) 17:00까지 도착분에 한함
+ - 제출장소: (우: 47340) 부산광역시 부산진구 엄광로 176, 동의대학교 입학관리팀
+ 추가사항
+ - 검정고시출신자 및 외국고교 졸업(예정)자의 제출서류 중 학교생활기록부 대체 서류는 선택 제출서류로 ‘학교생활기록부 대체 서류’ 양식을 참조.
+ 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>평생학습자전형은 대학에서 평생교육을 받은 학습자를 선발하기 위한 전형입니다. 주요 특징과 지원 자격, 제출 서류 등을 다음과 같이 요약할 수 있습니다:
+### 주요 특징:
+1. **지원 자격**: 고교 졸업(예정)자 또는 법령에 의한 동등학력 소지자.
+2. **재직 기간**: 4대 보험 중 1개 이상 가입 사업체에서 재직 중인 경우, 2024년 3월 1일 기준 총 재직기간이 3년 이상이어야 합니다.
+3. **전형 요소 반영 비율**: 서류 평가 70%, 면접 평가 30%로 구성됩니다.
+### 제출 서류:
+- **고교 졸업(예정)자**:
+  - 고교 학교생활기록부 1부 (학생부 온라인 제공 동의자는 제출할 필요 없음)
+- **검정고시 출신자**:
+  - 검정고시 합격증서 사본 또는 합격증명서 1부
+  - 검정고시 성적증명서 1부 (온라인 제공 동의자는 제출할 필요 없음)
+  - 학교생활기록부 대체 서류(제출 여부 선택 가능)
+- **외국고교 졸업(예정)자**:
+  - 공증받은 외국고교 졸업(예정)증명서 1부
+  - 공증받은 외국고교 성적증명서 1부 (만점이 명시된 고교성적 체계자료를 성적증명서 뒤에 첨부해야 함)
+  - 학교생활기록부 대체 서류(제출 여부 선택 가능) (외국어로 작성된 경우, 원본과 공증받은 한국어 번역본을 함께 제출해야 함)
+### 추가 정보:
+- **면접 평가**: 개별 면접으로 진행되며, 1인당 10분 이내입니다.
+- **서류 제출 기간 및 장소**:
+  - 제출기간: 2024년 1월 3일(수) ~ 12일(금) 17:00까지 도착분에 한함
+  - 제출장소: (우: 47340) 부산광역시 부산진구 엄광로 176, 동의대학교 입학관리팀
+평생학습자전형은 평생교육을 받은 학습자의 역량과 노력에 중점을 둔 전형으로, 서류와 면접 모두에서 학생들의 개인적 성장과 노력이 중요하게 평가됩니다.</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>0.6126741120001052</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>평생학습자전형의 지원자격은 다음과 같습니다
+ - 고교 졸업(예정)자 또는 법령에 의한 동등학력 소지자</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>평생학습자전형의 지원 자격은 다음과 같습니다:
+1. 고교 졸업(예정)자 또는 법령에 의한 동등학력 소지자
+2. 만 30세 이상인 자 (1994년 2월 28일 이전 출생자)
+이러한 조건을 만족하는 지원자가 해당 전형의 지원 자격을 갖추게 됩니다.</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>0.2320772071263408</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>실기고사 대기실 및 입실시간은 2024. 01. 12.(금) 14:00 이후 입학안내 홈페이지에서 조회 가능합니다.</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 실기고사에 대한 정보는 다음과 같습니다:
+1. **레저스포츠학과**:
+   - 실기종목: 제자리 멀리뛰기, Z-런
+   - 장소: 해당 학과에서 실시
+2. **태권도학과**:
+   - 실기종목 및 배점: 기초실기 200점(20%), 응용실기 500점(50%)
+   - 장소: 해당 학과에서 실시
+3. **디자인조형학과 (시각디자인, 산업디자인, 공예디자인)**:
+   - 실기종목 및 배점: 기초디자인 700점(70%)
+   - 장소: 해당 학과에서 실시
+4. **체육학과**:
+   - 실기종목 및 배점: 제자리 멀리뛰기 240점(24%), 메디신볼 던지기 243점(23%), Z-런 230점(23%)
+   - 장소: 해당 학과에서 실시
+실제 시험장소는 각 모집단위별로 다를 수 있으므로, 정확한 장소와 기타 세부 사항은 해당 학과의 공지사항이나 입학관리팀에 문의하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>0.0004880442036259545</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>실기고사 대기실 및 입실시간은 2024. 01. 12.(금) 14:00 이후 입학안내 홈페이지에서 조회 가능합니다.</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>2024년 체육학과의 실기고사는 다음과 같이 진행됩니다:
+- **일정**: 2024. 01. 16.(화)
+- **대기실 및 입실시간 안내**: 2024. 01. 12.(금) 14:00 이후, 입학안내 홈페이지에서 조회 가능
+따라서 체육학과의 실기고사는 2024년 1월 16일 화요일에 진행되며, 이 날짜 전날인 1월 12일 금요일 오후 2시 이후부터 대기실 및 입실 시간 안내를 확인할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D315" t="n">
+        <v>0.06935053649302352</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>아니요, 수시 충원합격자 발표는 전화로 개별 연락을 하지 않습니다. 최초합격자 및 1차, 2차 충원합격자 발표는 홈페이지를 통해 실시하며, 모든 지원자는 전형 일정에 명시된 합격자 발표일에 합격 여부를 반드시 홈페이지를 통해 확인해야 합니다. 3차 이후 충원합격자 발표 과정에서만 개별 전화 통보가 이루어집니다.</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>2024년 2월 15일(목)부터 2024년 2월 20일(화)까지 충원합격자를 발표할 때, 전화 연락 두절로 인해 충원합격 통보가 어려운 경우, 충원합격이 되었으나 등록 의사가 없는 등록 포기자로 간주하므로, 이 기간 동안 전화 연락을 받지 못하는 일이 없도록 유의하시기 바랍니다.
+따라서, 수시 충원합격자 발표 시 별도로 전화를 주지는 않을 것으로 보입니다. 지원자는 이 기간 동안 합격 여부를 홈페이지에서 확인하고, 필요하다면 입학관리팀에 연락하여 확인하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>0.2686501443319728</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>제공된 정시 모집요강에는 2023학년도 경찰행정학과 수시모집 결과에 대한 정보가 포함되어 있지 않습니다. 해당 정보를 확인하려면 "https://ipsi.deu.ac.kr/main.do"를 방문하여 문의하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>2023학년도 경찰행정학과의 수시모집 결과에 대한 정보가 제공된 문서에서는 직접적으로 언급되어 있지 않습니다. 해당 학과에 대한 모집인원이나 최종합격자 등 구체적인 수시모집 결과는 제공되지 않았습니다.
+문서에서 경찰행정학과 관련하여 확인할 수 있는 정보는 다음과 같습니다:
+- 2024학년도에는 경찰행정학과가 모집단위에 포함되어 있지 않습니다 (나군 학생부교과(농어촌학생전형) - 정원외 모집단위 및 모집인원 표에서 확인 가능).
+따라서, 2023학년도 경찰행정학과의 수시모집 결과를 찾으려면 동의대학교 입학처 웹사이트나 관련 공지사항을 확인해 보는 것이 좋겠습니다. 해당 정보가 올바르게 기재되어 있지 않다면 대학 입학처에 직접 문의하는 것도 방법입니다.</t>
+        </is>
+      </c>
+      <c r="D317" t="n">
+        <v>0.06690107015324646</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>아니요, 정시모집 지원자는 수능에 응시하지 않으면 지원할 수 없습니다.</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>2024년 동계학기 정시모집에서 수능을 응시하지 않은 학생들도 지원이 가능합니다. 그러나 수능 성적은 일부 전형에서 중요한 평가 요소로 사용되므로, 수능 응시를 권장드립니다.
+특히 다음과 같은 전형에서는 수능 성적이 반영됩니다:
+1. **나군 실기/실적(일반학생전형)**: 디자인조형학과, 체육학과, 레저스포츠학과, 태권도학과 등에서 수능 성적이 35,000원의 전형료와 함께 반영됩니다.
+2. **나군 학생부교과(농어촌학생전형)**: 이 전형에서는 수능은 필요하지 않지만, 지원 자격을 갖추기 위해 농어촌 지역 거주 기록 등이 요구됩니다.
+3. **나군 학생부종합(평생학습자전형), 성인학습자(정원내/외)전형, 재직자전형, 조기취업형계약학과전형**: 이들 전형에서는 수능 성적이 아닌 다른 평가 기준이 주로 사용되므로 수능 응시는 필요하지 않습니다.
+하지만, 수능 성적은 학력 확인 및 입학성적 평가에 중요한 역할을 하므로, 가능하다면 수능을 응시하는 것이 좋습니다. 특히 일반학생전형의 경우, 수능 성적이 전형 점수 계산에 포함되므로 이를 고려해보세요.
+더 자세한 정보는 동의대학교 입학관리 홈페이지를 참조하시거나 학교 관계자에게 문의하시는 것을 권장드립니다.</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>2.500181069383438e-07</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>네, 고등학교 졸업한지 10년이 지났더라도 정시 지원이 가능합니다. "고교유형별 지원자격" 표에 따르면, 일반고, 자율고, 특수목적고, 특성화고, 영재학교, 기타 학교, 검정고시, 외국고 출신자 모두 정시 지원이 가능합니다. 따라서 고등학교 졸업 시기와 상관없이 지원할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 일반적으로 대학의 정시모집에서는 고등학교를 졸업한 후 3년 이상 경과하면 지원 자격이 제한될 수 있습니다. 하지만 특정 전형에 따라 예외적인 경우도 있을 수 있습니다.
+주어진 정보로는 다음과 같은 점을 확인할 수 있습니다:
+1. **나군 학생부종합(평생학습자전형)**: 이 전형은 고등학교 졸업(예정)자 또는 법령에 의한 동등학력 소지자를 대상으로 합니다.
+2. **성인학습자(정원내·외)전형**: 이 전형도 고등학교 졸업(예정)자 또는 법령에 의한 동등학력 소지자로서 만 30세 이상인 자를 대상으로 합니다 (1994년 2월 28일 이전 출생자).
+3. **재직자전형**: 이 전형은 「고등교육법 시행령」 제29조 제2항 제14호 '다'목에 해당하는 자를 대상으로 합니다 (즉, 산업체 근무경력이 3년 이상인 재직자).
+따라서 고등학교 졸업한지 10년이 지났다면, 다음과 같은 전형을 통해 지원할 수 있을 가능성이 있습니다:
+- **평생학습자전형**: 이는 고등학교 졸업(예정)자를 대상으로 하므로 적합합니다.
+- **성인학습자(정원내·외)전형**: 만 30세 이상이면 지원할 수 있습니다.
+하지만 일반적인 정시모집에서는 이러한 기간 경과로 인해 지원 자격이 제한될 가능성이 높습니다. 특정 대학이나 전형의 세부 조건을 확인하시거나, 해당 대학 입학처에 문의하시는 것이 가장 확실합니다.
+더 자세한 정보를 얻기 위해서는 [https://ipsi.deu.ac.kr/main.do](https://ipsi.deu.ac.kr/main.do) 웹사이트를 참조하거나, 동의대학교 입학관리팀으로 연락하시면 도움을 받으실 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>0.007012058118751662</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>동의대학교의 2024학년도 정시 일정은 다음과 같습니다
+1. 모집인원 확정 공고
+   - 일정: 2024년 1월 2일(화)
+   - 비고: 입학안내 홈페이지 공고
+2. 원서접수(인터넷)
+   - 일정: 2024년 1월 3일(수) ~ 2024년 1월 6일(토) 마감일 18시까지
+   - 비고: http://ipsi.deu.ac.kr 또는 http://www.uwayapply.com
+3. 서류 제출 (제출서류가 있는 경우)
+   - 일정: 2024년 1월 3일(수) ~ 2024년 1월 12일(금) 마감일 17시까지 도착
+   - 비고: 서류 제출대상 (Ⅳ. 전형별 세부 안내 참조)
+   - 제출방법: 접수사이트에서 우편발송용 표지를 출력하여 부착 후 제출 또는 우편발송
+4. 실기고사
+   - &lt;가&gt;군 실기고사 레저스포츠학과 태권도학과
+     - 일정: 2024년 1월 16일(화)
+     - 비고: 대기실 및 입실시간 안내 2024년 1월 12일(금) 14:00 이후 입학안내 홈페이지에서 조회
+   - &lt;나&gt;군 실기고사 디자인조형학과 (시각디자인, 산업디자인, 공예디자인) 체육학과
+     - 일정: 2024년 1월 17일(수)
+     - 비고: 대기실 및 입실시간 안내 2024년 1월 12일(금) 14:00 이후 입학안내 홈페이지에서 조회
+5. 합격자 발표 및 등록금 납부
+   - 최초 합격자 발표
+     - 일정: 2024년 2월 2일(금) 14:00
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+   - 최초 합격자 등록
+     - 일정: 2024년 2월 7일(수) ~ 2월 13일(화) (은행마감시간 내)
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+   - 충원 합격자 1차 (인터넷) 발표
+     - 일정: 2024년 2월 14일(수) 09:00
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+   - 충원 합격자 1차 (인터넷) 등록
+     - 일정: 2024년 2월 14일(수) 09:00 ~ 16:00
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+   - 충원 합격자 2차 (인터넷) 발표
+     - 일정: 2024년 2월 15일(목) 09:00
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+   - 충원 합격자 2차 (인터넷) 등록
+     - 일정: 2024년 2월 15일(목) 09:00 ~ 16:00
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+   - 충원 합격자 3차 이후 (개별 전화 통보) 발표
+     - 일정: 2024년 2월 15일(목) 19:00 ~ 2024년 2월 20일(화) 18시까지
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+   - 충원 합격자 3차 이후 (개별 전화 통보) 등록
+     - 일정: 개별 전화 통보 시 안내
+     - 비고: 홈페이지에서 개별 조회, 고지서 교부: 홈페이지에서 출력 또는 입학관리팀에서 수령, 등록장소: 학교 지정은행(등록금 고지서에 기재)
+추가 유의사항:
+- 최초합격자 및 1차, 2차 충원합격자 발표는 홈페이지를 통해 실시하며, 모든 지원자는 전형일정에 명시된 합격자 발표일에 합격 여부를 홈페이지를 통해 확인해야 합니다. 별도 개별 연락을 실시하지 않으며, 합격 여부 미확인으로 인해 등록하지 못했다 하더라도 등록(입학) 포기자로 간주합니다.
+- 최초 및 충원합격자는 전형일정에 명시된 등록 일정을 참고하여 지정 기일 내에 등록금을 납부해야 하며, 지정 기일 내에 등록금을 납부하지 않는 경우 입학을 포기하는 것으로 간주합니다.</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>동의대학교 정시 모집의 주요 일정은 다음과 같습니다:
+1. **모집인원 확정 공고**: 2024년 1월 2일 (화)
+   - 입학 안내 홈페이지에서 공고됩니다.
+2. **원서접수(인터넷)**: 2024년 1월 3일 (수) ~ 2024년 1월 6일 (토), 마감 시간은 각 날짜별로 오후 6시까지입니다.
+   - 접수 사이트는 [http://ipsi.deu.ac.kr](http://ipsi.deu.ac.kr) 또는 [http://www.uwayapply.com](http://www.uwayapply.com)를 통해 가능합니다.
+3. **서류 제출 (제출서류가 있는 경우)**: 2024년 1월 3일 (수) ~ 2024년 1월 12일 (금), 마감 시간은 각 날짜별로 오후 5시까지 도착해야 합니다.
+   - 서류 제출 대상은 전형별 세부 안내를 참조해야 하며, 접수 사이트에서 우편발송용 표지를 출력하여 부착 후 제출하거나 우편으로 보내야 합니다.
+4. **&lt;가&gt;군 실기고사 (레저스포츠학과, 태권도학과)**: 2024년 1월 16일 (화)
+   - 대기실 및 입실 시간 안내는 2024년 1월 12일 (금) 오후 2시 이후에 입학 안내 홈페이지에서 확인 가능합니다.
+5. **&lt;나&gt;군 실기고사 (디자인조형학과, 체육학과)**: 2024년 1월 17일 (수)
+   - 대기실 및 입실 시간 안내는 2024년 1월 12일 (금) 오후 2시 이후에 입학 안내 홈페이지에서 확인 가능합니다.
+6. **합격자 발표 및 등록금 납부**:
+   - 최초 합격자 발표: &lt;가&gt;군, &lt;나&gt;군, &lt;다&gt;군 2024년 2월 2일 (금) 오후 2시
+     - 홈페이지에서 개별 조회 가능하며, 고지서 교부는 홈페이지에서 출력하거나 입학관리팀에서 수령 가능합니다.
+   - 최초 합격자 등록: 2024년 2월 7일 (수) ~ 2024년 2월 13일 (화), 은행 마감 시간 내에 이루어져야 합니다.
+     - 홈페이지에서 개별 조회 가능하며, 고지서 교부는 홈페이지에서 출력하거나 입학관리팀에서 수령 가능합니다.
+   - 충원 합격자 발표 및 등록: 
+     1차 (인터넷) 발표 및 등록: 2024년 2월 14일 (수) 오전 9시 ~ 오후 4시
+     2차 (인터넷) 발표 및 등록: 2024년 2월 15일 (목) 오전 9시 ~ 오후 4시
+     3차 이후 (개별 전화 통보): 2024년 2월 15일 (목) 오후 7시 ~ 2024년 2월 20일 (화) 오후 6시까지
+7. **합격자 발표 및 등록금 납부**:
+   - 충원 합격자는 지정 기간 내에 등록금을 납부해야 하며, 지정 기한 내에 납부하지 않으면 입학 포기로 간주됩니다.
+모든 지원자는 전형 일정에 명시된 합격자 발표일에 반드시 합격 여부를 확인해야 합니다. 또한, 최초 및 충원합격자는 등록 기간 내에 등록금을 납부해야 하며, 지정 기한 내에 납부하지 않으면 입학 포기를 간주됩니다.
+상세 일정과 추가 정보는 [입학 안내 홈페이지](http://ipsi.deu.ac.kr)를 참조하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>0.4771094381062614</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>동의대학교 정시 모집 일정은 다음과 같습니다:
+1. 모집인원 확정 공고: 2024년 1월 2일(화)에 입학안내 홈페이지에 공고됩니다.
+2. 원서접수(인터넷): 2024년 1월 3일(수)부터 2024년 1월 6일(토) 18시까지 진행됩니다. 접수는 [입학안내 홈페이지](http://ipsi.deu.ac.kr) 또는 [유웨이 어플라이](http://www.uwayapply.com)에서 가능합니다.
+3. 서류 제출 (제출서류가 있는 경우): 2024년 1월 3일(수)부터 2024년 1월 12일(금) 17시까지 도착해야 합니다. 서류 제출 대상자는 접수 사이트에서 우편발송용 표지를 출력하여 부착 후 제출하거나 우편으로 발송해야 합니다.
+4. 실기고사 일정:
+   - &lt;가&gt;군 실기고사: 레저스포츠학과, 태권도학과는 2024년 1월 16일(화)에 실시됩니다. 대기실 및 입실시간 안내는 2024년 1월 12일(금) 14:00 이후 입학안내 홈페이지에서 조회할 수 있습니다.
+   - &lt;나&gt;군 실기고사: 디자인조형학과(시각디자인, 산업디자인, 공예디자인), 체육학과는 2024년 1월 17일(수)에 실시됩니다. 대기실 및 입실시간 안내는 2024년 1월 12일(금) 14:00 이후 입학안내 홈페이지에서 조회할 수 있습니다.
+5. 합격자 발표 및 등록금 납부:
+   - 최초 합격자 발표: &lt;가&gt;군, &lt;나&gt;군, &lt;다&gt;군 모두 2024년 2월 2일(금) 14:00에 발표됩니다. 발표는 홈페이지에서 개별 조회할 수 있으며, 고지서는 홈페이지에서 출력하거나 입학관리팀에서 수령할 수 있습니다. 등록장소는 학교 지정은행입니다.
+   - 최초 합격자 등록: 2024년 2월 7일(수)부터 2월 13일(화)까지 은행 마감시간 내에 등록해야 합니다.
+   - 충원 합격자 발표 및 등록:
+     - 1차 발표: 2024년 2월 14일(수) 09:00, 등록은 같은 날 09:00~16:00
+     - 2차 발표: 2024년 2월 15일(목) 09:00, 등록은 같은 날 09:00~16:00
+     - 3차 이후 발표: 2024년 2월 15일(목) 19:00부터 2024년 2월 20일(화) 18:00까지 개별 전화 통보, 등록은 개별 전화 통보 시 안내됩니다.
+모든 지원자는 전형일정에 명시된 합격자 발표일에 홈페이지를 통해 합격 여부를 확인해야 하며, 지정 기일 내에 등록금을 납부하지 않으면 입학을 포기하는 것으로 간주됩니다.</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 정시 모집 일정은 다음과 같습니다:
+1. **모집인원 확정 공고**: 2024년 1월 2일 (화요일)
+2. **원서접수(인터넷)**: 
+   - 시작일: 2024년 1월 3일 (수요일)
+   - 마감일: 2024년 1월 6일 (토요일) 18시까지
+3. **서류 제출**:
+   - 시작일: 2024년 1월 3일 (수요일)
+   - 마감일: 2024년 1월 12일 (금요일) 17시까지 도착분에 한함
+4. **&lt;가&gt;군 실기고사**:
+   - 레저스포츠학과, 태권도학과: 2024년 1월 16일 (화요일)
+5. **&lt;나&gt;군 실기고사**:
+   - 디자인조형학과 (시각디자인, 산업디자인, 공예디자인): 2024년 1월 17일 (수요일)
+   - 체육학과: 2024년 1월 17일 (수요일)
+6. **합격자 발표 및 등록금 납부**:
+   - 최초 합격자 발표: 2024년 2월 2일 (금요일) 14시
+   - 최초 합격자 등록: 2024년 2월 7일 (수요일) ~ 2024년 2월 13일 (화요일)
+7. **충원 합격자 발표 및 등록**:
+   - 1차 충원 합격자 발표: 2024년 2월 14일 (수요일) 9시
+   - 1차 충원 합격자 등록: 2024년 2월 14일 (수요일) 9시 ~ 16시
+   - 2차 충원 합격자 발표: 2024년 2월 15일 (목요일) 9시
+   - 2차 충원 합격자 등록: 2024년 2월 15일 (목요일) 9시 ~ 16시
+   - 3차 이후 충원 합격자 발표 및 등록: 2024년 2월 15일 (목요일) 19시 ~ 2024년 2월 20일 (화요일) 18시까지
+이 일정은 일반적으로 지원자가 참고해야 하는 주요 날짜들입니다. 각 단계별로 합격 여부를 확인하고, 지정된 기간 내에 등록금을 납부하는 것이 중요합니다.</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>0.4945352845532207</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>동의대학교 정시 모집 전형에서는 수능 성적자료의 온라인 제공에 동의하는 것으로 간주되며, 수능 성적이 요구됩니다. 따라서 수능 미응시자는 지원이 불가능합니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 정시모집에서 수능을 미응시한 지원자가 지원할 수 있는 전형으로는 "학생부교과(농어촌학생전형)"와 "학생부종합(성인학습자(정원내)전형), 학생부종합(성인학습자(정원외)전형), 학생부종합(재직자전형), 학생부종합(조기취업형계약학과전형)" 등이 있습니다.
+특히, "학생부교과(농어촌학생전형)"는 수능을 미응시한 지원자가 지원할 수 있는 전형 중 하나로, 해당 모집단위에서는 수능 점수 대신 학생부 교과 성적을 주요 평가 기준으로 합니다.
+따라서 수능을 미응시한 지원자는 이러한 전형들을 통해 지원이 가능합니다.</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>0.1018250718789152</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>동의대학교 정시 모집 전형에는 충원 합격 차수에 대한 정보가 존재하지않습니다.
+전년도의 전자공학과의 충원 합격은 36명까지 이루어졌습니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>2024년의 전형 일정을 보면, 충원 합격자는 다음과 같이 발표되었습니다:
+- 1차 충원 합격자 발표: 2024. 02. 14.(수) 09:00
+- 2차 충원 합격자 발표: 2024. 02. 15.(목) 09:00
+따라서 전년도(2023년)의 전자공학과의 충원 합격은 최대 2차까지 이루어졌을 것으로 추정할 수 있습니다.
+하지만 정확한 정보를 얻기 위해서는 해당 대학의 입학처 웹사이트나 공지사항을 확인하는 것이 가장 확실합니다. 제공된 정보에 따르면, 충원 합격자는 3차 이후에는 개별 전화 통보로 이루어진다고 언급되어 있습니다.</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>0.1195294851563881</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>동의대학교 입학관리팀 연락처는 051-890-4379~89입니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>提供的信息中并没有直接提到东义大学入学处的电话号码。如果您需要联系东义大学入学处，建议您访问其官方网站（https://ipsi.deu.ac.kr/main.do），通常学校官网会有联系方式等重要信息。如果仍然无法找到相关信息，可以尝试通过网站上的在线咨询服务或发送电子邮件进行询问。
+希望这能帮助到您！如果有其他问题，请随时告诉我。</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>0.1506425879680184</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>3차 이후 충원합격자 발표 과정에서 전화 연락이 두절되어(3회 통화 시도) 충원합격 통보가 어려운 경우, 해당 지원자는 등록 의사가 없는 것으로 간주되어 등록 포기자로 처리됩니다. 따라서 충원합격자 발표 기간(2024년 2월 15일(목)~2024년 2월 20일(화)) 동안 전화 연락을 받을 수 있도록 유의해야 합니다.</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>3차 이후 충원합격자 발표 과정에서 전화 연락 두절(3회 통화)로 인해 충원합격 통보가 어려운 경우, 충원합격이 되었으나 등록 의사가 없는 것으로 간주됩니다. 따라서 지원자는 2024년 2월 15일(목)부터 2024년 2월 20일(화)까지 전화 연락을 받지 못하는 일이 없도록 유의해야 합니다.</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>0.7498341960216179</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>농어촌학생전형으로 지원 시 제출해야 할 서류는 다음과 같습니다
+6년 과정
+지원자 본인의 가족관계증명서 1부
+지원자 본인, 부, 모의 주민등록초본 각 1부 (총 3부)
+중학교 학교생활기록부 1부
+교육기관(초·중·고교), 공공기관, 무인민원발급기, 인터넷 정부24에서 발급
+고등학교 학교생활기록부 1부 (학생부 온라인 제공 비대상교 및 미동의자)
+부모가 사망한 경우: 사망한 부 또는 모의 기본증명서 1부 (기본증명서에 ‘사망’이 명시되어 있지 않은 경우 제적등본 1부 추가 제출)
+부모가 이혼한 경우: 친권이 있는 부 또는 모의 혼인관계증명서(상세) 1부, 본인의 기본증명서(상세) 1부 추가 제출
+12년 과정
+지원자 본인의 주민등록초본 1부
+초등학교 학교생활기록부 1부
+중학교 학교생활기록부 1부
+고등학교 학교생활기록부 1부 (학생부 온라인 제공 비대상교 및 미동의자)
+중·고등학교 재학 시 부, 모 모두 농어촌(읍·면)지역에서 거주한 자는 ‘6년과정' 서류 제출 가능
+교육기관(초·중·고교), 공공기관, 무인민원발급기, 인터넷 정부24에서 발급
+추가 정보
+제출기간: 2024. 01. 03.(수) ~ 01. 12.(금) 17:00까지 도착분에 한함
+제출장소: (우: 47340) 부산광역시 부산진구 엄광로 176, 동의대학교 입학관리팀
+주의사항: 제출서류 미제출자는 불합격 처리됩니다. 
+주민등록초본, 가족관계증명서, 혼인관계증명서, 기본증명서는 주민등록번호 전체가 기재되어 있어야 하며, 주소변동사항이 포함된 서류를 발급받아 제출하여야 합니다.
+상기 서류는 2024년 1월 1일 이후에 발급된 서류에 한해 제출해야 합니다. 
+최종등록자 중 고교 졸업예정자는 졸업 이후 지원자격 증빙서류를 2024. 02. 16.(금)까지 추가 제출하여야 합니다.</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>6년 과정과 12년 과정의 농어촌학생전형 지원을 위해서는 각각 다음과 같은 서류를 제출해야 합니다.
+### 6년 과정 (농어촌(읍·면)지역 소재 중·고등학교에서 전 교육과정을 이수한 자로서 중·고등학교 재학기간 중 본인 및 부모 모두가 농어촌(읍·면) 지역에 거주한 자)
+1. 지원자 본인의 가족관계증명서 1부
+2. 지원자 본인, 부, 모의 주민등록초본 각 1부 (총 3부)
+3. 중학교 학교생활기록부 1부 (교육기관, 공공기관, 무인민원발급기, 인터넷 정부24에서 발급 가능)
+4. 고등학교 학교생활기록부 1부 (학생부 온라인 제공 비대상 교 및 미동의자) 
+5. 부모가 사망한 경우, 사망한 부 또는 모의 기본증명서 1부 (기본증명서에 ‘사망’이 명시되어 있지 않은 경우 제적등본 1부)
+6. 부모가 이혼한 경우, 친권이 있는 부 또는 모의 혼인관계증명서(상세) 1부, 본인의 기본증명서(상세) 1부
+### 12년 과정 (부모의 거주지와는 상관없이 지원자 본인이 초·중·고등학교 전 교육과정을 농어촌(읍·면) 지역 소재 학교에서 이수하고 거주한 자)
+1. 지원자 본인의 주민등록초본 1부
+2. 초등학교 학교생활기록부 1부 
+3. 중학교 학교생활기록부 1부
+4. 고등학교 학교생활기록부 1부 (학생부 온라인 제공 비대상 교 및 미동의자)
+**추가 제출서류:**
+최종 등록자 중 고교 졸업예정자는 졸업 이후 지원자격 증빙서류를 2024년 2월 16일(금)까지 추가 제출해야 합니다.
+- 6년 과정: 고교 졸업증명서, 지원자 본인, 부, 모 초본 각 1부 (총 3부)
+- 12년 과정: 고교 졸업증명서, 지원자 본인 초본 1부
+**주의사항:**
+- 주민등록초본은 2024년 1월 1일 이후 발급된 서류에 한해 제출 가능합니다.
+- 주민등록초본은 주소변동사항이 포함된 서류를 발급받아 제출해야 합니다.</t>
+        </is>
+      </c>
+      <c r="D326" t="n">
+        <v>0.7257150014798393</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>농어촌학생전형으로 지원 시 12년 과정이 제출해야 할 서류는 다음과 같습니다
+1. 지원자 본인의 주민등록초본 1부
+2. 초등학교 학교생활기록부 1부
+3. 중학교 학교생활기록부 1부
+4. 고등학교 학교생활기록부 1부 (학생부 온라인 제공 비대상교 및 미동의자)
+추가로, 최종등록자라면 다음 서류도 제출해야 합니다
+1. 고교 졸업증명서
+2. 지원자 본인의 주민등록초본 1부 주민등록초본은 고교 졸업 이후 발급된 것이어야 하며, 주소변동사항이 포함된 서류를 발급받아 제출해야 합니다.</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>12년 과정의 농어촌학생전형 지원자는 다음과 같은 서류를 제출해야 합니다:
+- 지원자 본인의 주민등록초본 1부
+- 초등학교 학교생활기록부 1부 
+- 중학교 학교생활기록부 1부
+- 고등학교 학교생활기록부 1부(학생부 온라인 제공 비대상교 및 미동의자)
+추가적인 주의사항:
+- 제출기간은 2024. 01. 03.(수) ~ 01. 12.(금) 17:00까지 도착분에 한함
+- 제출장소는 (우: 47340) 부산광역시 부산진구 엄광로 176, 동의대학교 입학관리팀
+- 주민등록초본은 고교졸업 이후 발급되어야 하며, 주소변동사항이 포함된 서류를 발급받아 제출해야 합니다.
+- 상기 서류는 2024년 1월 1일 이후에 발급된 서류에 한해 제출 가능합니다.
+- 최종등록자 중 고교 졸업예정자는 졸업 이후 지원자격 증빙서류를 2024. 02. 16.(금)까지 추가 제출해야 합니다.
+이러한 서류들을 정확하게 준비하고 제출하는 것이 중요합니다.</t>
+        </is>
+      </c>
+      <c r="D327" t="n">
+        <v>0.3912864188392561</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>동의대학교 정시 모집 전형에는 기회균등 전형이라는 전형이 존재하지 않습니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>提供的信息中并没有明确提到是否在正选招生（정시모집）中进行低收入机会均等类型的录取。因此，根据给出的信息无法确定正选招生是否会包含针对低收入家庭的特殊录取计划。
+如果您需要了解这方面的详细信息，建议直接访问东国大学入学管理委员会的官方网站或联系其相关部门以获取最准确的信息。网站上的最新公告和指南通常会提供此类特定招生政策的详细说明。</t>
+        </is>
+      </c>
+      <c r="D328" t="n">
+        <v>0.0293254909074653</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>제공된 데이터에는 수능 최저등급에 대한 구체적인 절사 여부에 대한 정보가 포함되어 있지 않습니다. 따라서, 수능 최저등급에서 사탐 2 과목 평균산출 시 2.5등급이 나올 경우 절사 여부에 대한 정확한 정보를 확인하려면 입학안내 홈페이지(http://ipsi.deu.ac.kr)에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 등급 평균 산출 시 소수점 셋째 자리에서 절사 처리한다는 내용이 포함되어 있습니다. 따라서 사탐 2과목의 평균을 계산할 때, 2.5등급은 소수점 셋째자리까지 반올림 후 절사됩니다.
+따라서 2.5등급은 3등급으로 반올림 후 절사되어 처리될 것입니다.
+이를 참고하여 수능 성적 평균을 계산하시면 됩니다.</t>
+        </is>
+      </c>
+      <c r="D329" t="n">
+        <v>0.309794124221845</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>정시 충원 합격자 발표는 3차까지 있으며, 3차 이후에는 개별 전화 통보로 발표됩니다. - 1차 발표: 2024. 02. 14.(수) 09:00 - 2차 발표: 2024. 02. 15.(목) 09:00 - 3차 이후 발표: 2024. 02. 15.(목) 19:00 ~ 2024. 02. 20.(화) 18시까지 3차 이후 발표는 개별 전화 통보로 진행됩니다.</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 정시 모집에서 충원 합격자는 다음과 같이 발표됩니다:
+1. **1차 충원 합격자 발표 및 등록**: 
+   - 날짜: 2024년 2월 14일(수) 09:00
+   - 방법: 홈페이지에서 개별 조회
+2. **2차 충원 합격자 발표 및 등록**: 
+   - 날짜: 2024년 2월 15일(목) 09:00
+   - 방법: 홈페이지에서 개별 조회
+3. **3차 이후 충원 합격자 발표 (개별 전화 통보)**:
+   - 날짜: 2024년 2월 15일(목) 19:00 ~ 2024년 2월 20일(화) 18시까지
+   - 방법: 홈페이지에서 개별 조회
+따라서, 정시 충원 합격자는 최대 3차까지 발표가 있을 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D330" t="n">
+        <v>0.2951088506960366</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>제공된 컨텍스트에 따라 e-비즈니스학과(e-비즈니스학과)의 최초 합격자 및 최종 등록생의 평균 점수는 다음과 같습니다:
+- 최초합격자:
+  - 국어 + 수학 + 탐구(2개) (가산점 포함) 표준 환산 점수 합: 317.20 (평균)
+  - 영어 등급 3.20 (평균)
+  - 수능 4개 영역 등급 4.17 (평균)
+  - 수능 4개 영역 (가산점 포함) 표준 변환 점수 합: 438.60 (평균)
+- 최종 등록 학생:
+  - 국어 + 수학 + 탐구(2개) (가산점 포함) 표준 변환 점수 합: 308.58 (평균)
+  - 영어 등급 3.66 (평균)
+  - 수능 4개 영역 등급 4.53 (평균)
+  - 수능 4개 영역 (가산점 포함) 표준 변환 점수 합: 426.25 (평균)
+수능 4개 영역 등급이 4.6점이라면 최초 합격자(4.17점)와 최종 등록자(4.53점) 모두 평균을 약간 상회하는 수준입니다. 반드시 합격이 보장되는 것은 아니지만 다른 영역(국어, 수학, 탐구, 영어) 성적이 경쟁력이 있다면 충원 합격(추가모집)을 통해 합격할 가능성이 있습니다. 
+보다 정확한 평가를 위해 총 표준 변환 점수 합과 제공된 평균을 비교하는 것이 좋습니다. 총점이 평균에 근접하거나 그 이상이면 충원 합격을 통해 합격할 가능성이 더 높을 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>4.6이라는 점수는 영어 등급에 해당합니다. 수능 영어 등급을 확인해보겠습니다.
+영어 등급별 점수표를 보면:
+- 1등급 : 139점
+- 2등급 : 131점
+- 3등급 : 123점
+- 4등급 : 115점 (이 경우 4.6)
+- 5등급 : 107점
+- 6등급 : 99점
+- 7등급 : 91점
+- 8등급 : 83점
+- 9등급 : 75점
+따라서 4.6은 4등급에 해당합니다.
+다군 수능(일반학생전형)의 경우, 수능 영어영역 등급에 따른 점수를 반영하며, 이는 합격 기준 중 하나입니다. 하지만 정시 전형으로 추가 합격 가능 여부는 단순히 영어 성적이 4등급이라는 것만으로는 판단하기 어렵습니다.
+다군 수능(일반학생전형)의 경우, 다음과 같은 점수를 반영합니다:
+- 국어 표준점수
+- 수학 표준점수
+- 영어 등급에 따른 점수 (이 경우 115점)
+- 탐구 표준점수
+따라서, 국어와 수학, 탐구 영역의 성적과 함께 영어 4등급의 점수를 합산하여 모집단위별 최저합격선을 충족하는지 확인해야 합니다.
+예를 들어, 인문사회과학대학의 경우:
+- 국어 표준점수
+- 수학 표준점수 (미적분 또는 기하)
+- 영어 4등급 점수 (115점)
+- 탐구 표준점수
+이 중에서 최저합격선을 충족하는지 확인해야 합니다. 만약 해당 모집단위의 최저합격선이 국어, 수학, 탐구 등 다른 영역에서도 높다면, 4등급만으로는 추가 합격하기 어렵다고 볼 수 있습니다.
+따라서, 정확한 답변을 위해서는:
+1. 해당 모집단위의 최저합격선을 확인해야 합니다.
+2. 국어와 수학, 탐구 영역의 성적도 함께 고려해야 합니다.
+이 정보를 바탕으로 추가 합격 가능성을 판단할 수 있습니다. 더 자세한 정보는 입학처 홈페이지나 전화로 문의하시는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D331" t="n">
+        <v>0.2820422156261947</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>e비즈니스학과의 최종등록자 데이터를 기준으로 보면, e비즈니스학과의 영어 등급 평균은 3.66이고, 수능 4개 영역 등급 평균은 4.53입니다. 따라서, 현재 정시 등급이 5.3이라면 e비즈니스학과에 합격하기 어려울 수 있습니다. e비즈니스학과의 평균 등급보다 높은 성적을 가지고 있어야 합격 가능성이 높아집니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 e비즈니스학과의 모집요강을 바탕으로, 정시 등급 5.3으로 최초합격 가능성을 평가해보겠습니다.
+1. **모집인원 및 전형 요소 반영 비율**:
+   - e비즈니스학과는 &lt;나&gt;군에 속하며, 전형요소 반영 비율은 수능 0%, 실기 30%입니다.
+2. **수능 등급**:
+   - 정시 등급 5.3은 상당히 낮은 등급이며, 이는 e비즈니스학과의 수능 점수 기준을 충족시키지 못합니다.
+3. **실기 성적**:
+   - 실기 성적이 중요하며, 실기 성적에 따라 합격 여부가 결정됩니다.
+   - e비즈니스학과는 실기 성적이 30%의 비율로 반영되므로, 실기 성적이 높은 지원자들이 선발될 가능성이 큽니다.
+4. **합격 가능성**:
+   - 정시 등급 5.3으로 e비즈니스학과에 최초 합격하기는 어렵습니다.
+   - 이 등급으로는 수능 점수 기준을 충족시키지 못하므로, 실기 성적이 매우 높아야 최초합격 가능성은 조금 있습니다.
+따라서 정시 등급 5.3으로 e비즈니스학과에 최초 합격하기는 어렵다고 판단됩니다. 실기 성적을 포함한 전반적인 경쟁력을 고려해야 합니다. 자세한 정보는 동의대학교 입학처 웹사이트를 참조하시거나, 입학처에 직접 문의하시는 것이 좋습니다.
+더 궁금하신 점이 있으시면 언제든지 물어보세요!</t>
+        </is>
+      </c>
+      <c r="D332" t="n">
+        <v>0.08047913367157616</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>e비즈니스학과의 최종등록자 데이터를 기준으로 보면, 충원합격(후보 순위) 31번까지 충원합격 된 것으로 나온다. 따라서, 현재 예비 38번이라면 e비즈니스학과에 예비 합격할 가능성이 낮습니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>提供的信息中没有关于e비즈니스학전공(电子商务学专业)的具体录取标准和分数线。因此，仅凭“预审38号”这一信息无法判断是否有可能被预录取。
+为了更准确地评估您是否有资格被预录取，建议参考以下几点：
+1. **查看最新的招生简章**：通常学校会在官网发布详细的招生简章，其中会包含各个专业的具体录取标准和分数线等信息。
+2. **了解专业要求**：电子商务学专业一般会有一定的学术成绩要求、英语水平要求等。请确保您的成绩单符合这些要求。
+3. **咨询学校**：直接联系学校的招生办公室或相关院系，询问具体的预录取情况和后续步骤。
+如果您能提供更多关于您个人成绩和其他相关信息（如GPA、英语考试成绩等），我可以帮助进一步分析。建议尽快访问学校官网获取最新信息，并与相关部门取得联系确认具体情况。</t>
+        </is>
+      </c>
+      <c r="D333" t="n">
+        <v>0.03539046323438171</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>간호학과의 최종등록자 데이터를 기준으로 보면, 간호학과의 영어 등급 평균은 2.34이고, 수능 4개 영역 등급 평균은 3.37입니다. 따라서, 현재 정시 등급이 3.44이라면 간호학과에 합격하기 어려울 수 있습니다. 간호학과의 평균 등급보다 높은 성적을 가지고 있어야 합격 가능성이 높아집니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>3.44이라는 GPA는 동의대학교 간호학과에 지원하는 데 있어 상대적으로 낮은 점수입니다. 하지만 합격 가능성 여부는 여러 요소로 결정됩니다:
+1. **전체 입시 경쟁률**: 동의대학교 간호학과의 경쟁률이 매우 높습니다. 2023년도에 6:1의 경쟁률을 기록했으며, 이는 매우 치열한 경쟁을 의미합니다.
+2. **학생부 평가**: GPA 외에도 학생부 평가 영역에서 좋은 성적을 받은 경우 합격 가능성은 높아집니다. 특히 공동체역량과 전공적합성 등이 중요하게 평가됩니다.
+3. **면접 성적**: 면접에서도 좋은 점수를 받는 것이 유리합니다. 일부 모집단위에서는 면접 점수가 합격 결정에 큰 영향을 미칩니다.
+4. **추천서 및 특기사항**: 추천서나 특기사항 등이 있다면 이도 긍정적으로 작용할 수 있습니다.
+5. **추가 지원 자격**: 일부 모집단위에서는 추가 지원 자격이나 경험이 유리하게 작용할 수 있으므로, 해당 부분을 확인해 보세요.
+6. **동점자 처리 기준**: 동점자가 발생했을 때의 처리 기준도 고려해야 합니다. 면접 성적이 높다면 이 점이 합격 결정에 영향을 미칠 수 있습니다.
+결론적으로, 3.44라는 GPA로는 매우 낮은 확률로 합격할 수 있지만, 다른 평가 요소들이 긍정적이라면 합격 가능성은 열려있습니다. 전반적인 지원 자질과 경쟁력을 고려하여 최선을 다해 준비하는 것이 중요합니다.
+추가적으로, 동의대학교 입학 홈페이지나 관계부서에 문의하시거나, 입시 상담을 받는 것도 도움이 될 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D334" t="n">
+        <v>0.03252787925079695</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>간호학과의 최종등록자 데이터를 보면, 평균 영어 등급은 2.34이고,  수능 4개 영역 등급 평균은 3.37입니다. 
+따라서, 현재 정시 등급이 2.52이라면 간호학과의 평균 등급보다 높은 성적을 가지고 있기 때문에 합격 가능성이 높습니다. 
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 간호학과의 모집인원과 지원 인원, 경쟁률을 살펴보겠습니다.
+- **모집인원**: 22명
+- **지원 인원**: 145명
+- **경쟁률**: 약 6.59대 1
+간호학과는 상당히 높은 경쟁률을 보이는 학과입니다. 평균적인 수능 점수를 보면, 최종합격자들의 국어 + 수학 + 탐구(2개) 표준 변환 점수 평균이 481.70점으로 매우 높습니다.
+당신의 성적이 2.52라면, 이는 표준변환점수로 환산하면 대략 300점대 중반에서 후반 정도가 됩니다. 이 점수가 간호학과의 평균적인 최종합격 점수(481.70점)와 비교해보면, 매우 낮은 수준입니다.
+따라서, 현재로서는 2.52라는 성적로 동의대학교 간호학과에 최종 합격하기는 어려울 것으로 보입니다. 하지만 입시 상황이 변동될 수 있으므로, 정확한 결과를 확인하려면 공식 발표를 기다리는 것이 좋습니다.
+추가적으로, 면접 등 다른 평가 요소도 고려해야 하며, 학생부 종합평가에서도 좋은 점수를 받는다면 가능성이 조금은 높아질 수 있습니다. 하지만 현재로서는 낮은 성적로 최종 합격하기는 어려울 것으로 예상됩니다.</t>
+        </is>
+      </c>
+      <c r="D335" t="n">
+        <v>0.05569395134480666</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>간호학과의 최종등록자 데이터를 기준으로 보면, 간호학과의 영어 등급 평균은 2.34이고, 수능 4개 영역 등급 평균은 3.37입니다. 따라서, 현재 정시 등급이 3.7이라면 간호학과의 평균 등급보다 낮은 성적을 가지고 있기 때문에 합격 가능성이 낮습니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>3.7의 성적은 중간적인 점수로, 간호학과에 합격하기 위해서는 여러 요소를 고려해야 합니다.
+1. **모집인원 및 경쟁률**: 간호학과의 모집인원과 해당년도의 경쟁률을 확인해야 합니다. 경쟁률이 높다면, 3.7의 성적만으로 합격하기는 어렵습니다.
+2. **전형요소 반영비율**: 나군 수능(일반학생전형)에서는 전 모집단위에서 수능성적이 100% 반영됩니다. 따라서 수능 점수가 중요한 역할을 합니다.
+3. **개인 성적 등급**: 나군의 경우, 학생부교과성적은 반영되지만 주요한 요소는 수능 성적입니다. 3.7의 성적은 중간등급으로, 경쟁률이 높다면 이만한 점수로 합격하기 어렵습니다.
+4. **추천서 및 자기소개서 등 서류평가**: 일부 전형에서는 추천서나 자기소개서 등의 서류평가가 이루어지므로, 이러한 부분에서 우수한 평가를 받는 것도 중요합니다.
+5. **면접 성적 (만약 필요하다면)**: 면접에서도 좋은 점수를 받는 것이 유리할 수 있습니다.
+6. **추천사**: 특정 학교나 모집단위에서는 추천사를 요구하거나 고려하므로, 이에 대한 준비도 필요합니다.
+결론적으로 3.7의 성적만으로 간호학과에 확실하게 합격하기는 어렵습니다. 경쟁률이 높다면 추가적인 지원 자료와 면접 등에서 우수한 평가를 받는 것이 중요합니다. 또한, 모집인원과 경쟁률을 확인하여 더 정확한 판단을 내리시길 바랍니다.
+추천: 
+- 해당년도의 간호학과 모집인원과 경쟁률을 확인하세요.
+- 전형요소 반영비율을 확인하고, 수능 성적이 주요한 역할을 하는지 파악하세요.
+- 추가 지원 자료와 면접 준비를 철저히 하세요.</t>
+        </is>
+      </c>
+      <c r="D336" t="n">
+        <v>0.01510371651716625</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>간호학과의 최종등록자 데이터를 기준으로 보면, 간호학과의 영어 등급 평균은 2.34이고, 수능 4개 영역 등급 평균은 3.37입니다. 따라서, 현재 정시 등급이 2.58이라면 간호학과의 평균 등급보다 높은 성적을 가지고 있기 때문에 합격 가능성이 높습니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 간호학과의 정시 모집에서는 수능 점수뿐만 아니라 학생부 성적, 면접 등 다양한 평가 요소들이 고려됩니다. 따라서 단순히 수능 점수만으로는 합격 여부를 판단하기 어렵습니다.
+간호학과의 경우 일반적으로 다음과 같은 평균적인 기준이 있습니다:
+1. **수능 성적**: 대체로 2.58 이상은 충분하지 않을 가능성이 높습니다. 간호학과는 보통 3.0 이상의 수능 점수가 요구됩니다.
+2. **학생부 성적**: 학생부 교과성적이 중요합니다. 특히 인성, 진로선택과목 등이 반영되므로 좋은 성적을 유지한 것이 유리합니다.
+3. **면접 성적**: 면접에서도 좋은 평가를 받는 것이 필요합니다. 간호사로서의 자질과 적합성을 잘 보여줘야 합니다.
+4. **추천서 등 추가 서류**: 일부 학교에서는 추천서나 자기소개서 등을 요구하기도 하므로 이에 대한 준비도 필요합니다.
+따라서, 수능 점수 2.58만으로는 간호학과에 정시로 합격하기 어렵다고 볼 수 있습니다. 하지만 학생부 성적, 면접 성적 등 다른 평가 요소들이 좋다면 합격 가능성은 열려있습니다.
+추천되는 조치:
+- **학생부 성적 확인**: 현재의 학생부 성적을 다시 한 번 점검하고 필요하다면 보강해야 합니다.
+- **면접 준비**: 면접 시 간호사로서의 자질과 적합성을 잘 보여줄 수 있도록 준비합니다.
+- **추천서 및 자기소개서 작성**: 필요한 경우 추천서와 자기소개서를 철저히 준비합니다.
+최종 합격 여부는 여러 평가 요소들이 복합적으로 고려되기 때문에, 정확한 판단을 위해서는 동의대학교 입학처 웹사이트나 전화로 상세 문의를 하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D337" t="n">
+        <v>0.01879259256712951</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>게임공학과의 최종등록자 데이터를 기준으로 보면, 충원합격(후보 순위) 3번까지 충원합격 된 것으로 나온다. 따라서, 현재 예비 7번이라면 게임공학과에 예비 합격할 가능성이 낮다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>为了回答您的问题，我需要查看相关的信息。根据您提供的数据表，游戏学（게임공학과）的招生名额为3人，并且有3个预录取名额（预备号码）。目前已经有3名学生被正式录取，所以您的预录取编号7是否能转正取决于学校是否有空缺名额。
+从表格中的信息来看，最终录取结果会根据多个因素决定，包括但不限于成绩、面试表现等。因此，虽然您是第7位预录取者，但并不保证一定能被录取。建议密切关注学校的官方通知和网站更新，以获取最新的录取信息。
+如果您想提高被录取的机会，可以：
+1. 确保您的学术成绩优异。
+2. 准备好参加可能的面试或其他评估环节，并表现出色。
+3. 关注学校发布的任何补充材料或额外要求的信息。
+希望这些信息对您有所帮助！如果有其他问题，请随时提问。</t>
+        </is>
+      </c>
+      <c r="D338" t="n">
+        <v>0.03234492933721011</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>게임공학과의 최종등록자 데이터를 기준으로 보면, 게임공학과의 영어 등급 평균은 3.25이고, 수능 4개 영역 등급 평균은 4.78입니다. 따라서, 현재 정시 등급이 4.16이라면 게임공학과의 평균 등급보다 높은 성적을 가지고 있어 합격 가능성이 높습니다. 단, 추가 합격 몇 번을 받을지는 예측하기 어렵습니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>4.16이라는 점수는 현재 수능 평균 점수와 비교했을 때 상대적으로 낮은 점수입니다. 동의대학교 게임공학과의 경우, 정시 전형에서 수능 성적에 크게 의존하는 경향이 있습니다.
+다만, 정확한 추가 합격 가능 횟수를 예측하기 위해서는 다음과 같은 요소들을 고려해야 합니다:
+1. **모집인원 및 지원자 수**: 동의대학교 게임공학과의 모집인원과 실제 지원자의 수에 따라 경쟁률이 달라질 수 있습니다.
+2. **경쟁률**: 현재 4.16이라는 점수로 지원하면, 해당 학과의 경쟁률을 고려해야 합니다. 경쟁률이 높다면 추가 합격 가능성은 낮아지게 됩니다.
+3. **전형별 특성**: 동의대학교는 다양한 전형(가군, 나군 등)으로 모집하므로, 지원자가 어떤 전형에 지원할 것인지에 따라 결과가 달라질 수 있습니다.
+4. **추가 합격 가능성**: 추가 합격 가능 횟수를 정확히 예측하기 어렵습니다. 경쟁률이 높다면 1차 합격 후 추가 합격을 받는 것이 어려울 수 있습니다.
+5. **개인 성적 향상**: 지원자가 수능 점수를 향상시키거나, 다른 전형(예: 실기/실적, 학생부종합 등)에서 우수한 성과를 거두면 추가 합격 가능성은 높아질 수 있습니다.
+따라서, 정확한 추가 합격 가능 횟수를 예측하기는 어렵습니다. 하지만 4.16이라는 점수로 지원한다면, 최소한의 경쟁률을 가지고 있는 전형에 지원하는 것이 유리할 것입니다. 또한, 다른 전형(실기/실적, 학생부종합 등)에서도 우수한 성과를 거두는 것이 중요합니다.
+추가 정보를 얻으시려면 동의대학교 입학처 웹사이트나 전화로 문의하시는 것을 추천드립니다.</t>
+        </is>
+      </c>
+      <c r="D339" t="n">
+        <v>0.03459014301896606</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>경영정보학과의 최초등록자 데이터를 기준으로 보면, 경영정보학과의 영어 등급 평균은 2.88이고, 수능 4개 영역 등급 평균은 3.88입니다.
+따라서, 현재 정시 등급이 3.75이라면 경영정보학과의 평균 등급보다 높은 성적을 가지고 있어 합격 가능성이 높습니다. 즉, 최초합격 가능성은 높아보입니다. 
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 정시모집에서 경영정보학과에 지원하려는 경우, 최초합격자의 합격 기준을 확인해야 합니다.
+주요 점은 다음과 같습니다:
+1. **성적 기준**: 경영정보학과의 경우, 수능 성적 3.75 이상이 필요합니다. 이는 대체로 중간 이상의 성적이어야 합니다.
+2. **최초합격자 발표 일정**: 최초합격자는 2024년 2월 2일(금)에 발표됩니다. 모든 지원자는 이날짜 이후 합격 여부를 확인해야 합니다.
+3. **등록 기간**: 최초합격자는 지정된 등록기간 내에 등록금을 납부해야 합니다 (2024년 2월 7일~13일).
+따라서, 경영정보학과의 정시 성적 기준이 3.75 이상이라면, 최초합격자로 선발될 가능성이 있습니다. 하지만 확실한 것은 최초합격자 발표 결과를 확인해야 합니다.
+**주의사항:**
+- 모든 지원자는 합격 여부를 반드시 홈페이지에서 확인해야 합니다.
+- 지정된 등록 기간 내에 등록금을 납부하지 않으면 입학이 포기됩니다.
+따라서, 최초합격자 발표 결과를 확인한 후 결정하시길 바랍니다. 더 자세한 정보는 동의대학교 입학관리 홈페이지를 참조하시거나 문의해보시는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D340" t="n">
+        <v>0.08640896823346196</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>경영정보학과의 최초등록자 데이터를 기준으로 보면, 경영정보학과의 영어 등급 평균은 2.88이고, 수능 4개 영역 등급 평균은 3.88입니다. 
+따라서, 현재 정시 등급이 4.2이라면 경영정보학과의 평균 등급보다 낮은 성적을 가지고 있어 합격 가능성이 낮습니다. 즉, 최초합격 가능성은 적습니다. 
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>为了回答这个问题，我们需要查看一些具体的信息。根据提供的信息，我们可以了解到：
+1. **招生类型和科目**：您提到的是“가군 수능(일반학생전형)”（即A类普通学生入学考试），这意味着主要依据高考成绩进行录取。
+2. **各专业具体的录取分数线**：虽然没有直接给出每个专业的具体分数线，但可以参考一般情况下，大多数本科专业的录取分数通常在400分以上。对于一些竞争激烈的热门专业，分数线可能会更高。
+3. **您的成绩**：您提到的“4.2”可能是指高考总分（满分100分），即42分。这个分数相对较低，不太可能达到一般本科专业的录取标准。
+因此，根据提供的信息和一般的招生情况，“4.2”的成绩在A类普通学生入学考试中通常不足以成为最初合格者（최초합격자）或补充合格者（충원합격자）。建议您查看具体专业的分数线或者直接咨询学校以获取更准确的信息。如果确实希望申请该专业，可能需要考虑其他类型的招生方式或其他大学的专业。
+如果您有更多关于特定专业的详细信息，比如具体的录取分数范围，请提供更多信息以便给出更精确的答案。</t>
+        </is>
+      </c>
+      <c r="D341" t="n">
+        <v>0.02736073645499888</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>경영정보학과의 최종등록자 데이터를 기준으로 보면, 경영정보학과의 영어 등급 평균은 3.25이고, 수능 4개 영역 등급 평균은 4.31입니다. 따라서, 현재 정시 등급이 5.33이라면 경영정보학과의 평균 등급보다 낮은 성적을 가지고 있어 합격 가능성이 낮습니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 경영정보학과의 경우, 수능(일반학생전형) 모집에 대한 정확한 합격 기준 점수는 공시되지 않았습니다. 하지만 일반적으로 대학별로 특정 학과에서의 최저합격선은 4.0 이상이 되어야 하는데, 일부 학과에서는 더 높은 점수가 요구될 수 있습니다.
+5.33이라는 표준점수는 상당히 좋은 성적입니다. 이 점수만으로는 확정적으로 합격 가능하다고 말하기 어렵습니다. 경영정보학과의 경우, 일반적으로 4.5 이상이 필요할 것으로 예상되지만, 최종 합격 가능성은 모집인원, 지원자들의 수능 성적 분포 등에 따라 달라질 수 있습니다.
+따라서, 다음과 같은 절차를 따르는 것이 좋습니다:
+1. **공식 정보 확인**: 동의대학교 입학 홈페이지나 공지사항을 통해 최신 합격 기준 점수와 모집인원 등을 확인하세요.
+2. **지원자 분석**: 지원자의 수능 성적과 경쟁률, 지원 인원 등을 고려하여 합격 가능성 평가를 해보세요.
+3. **추천서 및 서류 준비**: 필요하다면 추천서나 기타 서류를 준비하고 잘 작성하세요.
+만약 공식 정보에서 최저합격선이 4.5 이상이라면, 5.33이라는 점수는 충분히 경쟁력을 갖춘 것으로 볼 수 있습니다. 하지만 확실한 답변을 원한다면, 동의대학교 입학 홈페이지나 관계부서에 직접 문의하는 것이 가장 정확할 것입니다.
+[https://ipsi.deu.ac.kr/main.do](https://ipsi.deu.ac.kr/main.do)</t>
+        </is>
+      </c>
+      <c r="D342" t="n">
+        <v>0.04027392869522903</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>바이오응용공학부의 최초등록자 데이터를 기준으로 보면, 바이오응용공학부의 영어 등급 평균은 3.82이고, 수능 4개 영역 등급 평균은 4.74입니다. 
+따라서, 현재 정시 등급이 3.33이라면 바이오응용공학부의 평균 등급보다 높은 성적을 가지고 있어 합격 가능성이 높습니다. 즉, 최초합격 가능성은 있습니다. 
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>3.33이라는 GPA는 바이오응용공학부(의생명공학과, 바이오의약공학과, 식품공학과)에 지원하기에는 약간 낮은 점수일 수 있습니다. 하지만 최초등록자로 선발되는 것은 여러 요소가 작용합니다:
+1. **전형 유형**: 
+   - 학생부종합(평생학습자전형, 성인학습자전형, 재직자전형) 등에서 지원하면 GPA는 중요한 요인이지만, 다른 평가 기준도 중요합니다.
+2. **기타 평가 요소**:
+   - 학교생활기록부의 내용
+   - 면접 성과 (만약 면접이 포함된 전형이라면)
+   - 지원자의 특별한 경력이나 활동
+3. **전형 요소 반영 비율**:
+   - 학생부종합(평생학습자전형, 성인학습자전형, 재직자전형)은 서류 70%, 면접 30%로 구성되어 있습니다.
+4. **모집 단위별 특성**:
+   - 바이오응용공학부는 일반적으로 높은 학업 성적을 요구하지만, 평생학습자전형이나 재직자전형에서는 GPA가 조금 낮더라도 다른 요소를 보완할 수 있습니다.
+따라서 3.33의 GPA로 바이오응용공학부에 지원하려면:
+- **학교생활기록부**에서 높은 학업태도와 열정을 보여주어야 합니다.
+- **면접 성과**가 좋다면 이점을 활용할 수 있습니다.
+- **특별한 경력이나 활동**이 있다면 이를 강조해야 합니다.
+결론적으로, 3.33의 GPA로 최초등록자로 선발되는 것은 가능하지만, 다른 평가 요소들이 중요하게 작용합니다. 자세한 정보는 동의대학교 입학처 웹사이트를 참조하거나 직접 문의하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D343" t="n">
+        <v>0.04041015237159809</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>방사선학과의 최종등록자 데이터를 기준으로 보면, 방사선학과의 영어 등급 평균은 2.8이고, 수능 4개 영역 등급 평균은 3.82입니다. 
+따라서, 현재 정시 등급이 4.4이라면 방사선학과의 평균 등급보다 낮은 성적을 가지고 있어 합격 가능성이 낮습니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>4등급을 받으셨다면 방사선학과에 지원하는 것은 가능하지만, 경쟁률과 합격기준 등을 고려해야 합니다. 방사선학과는 일반적으로 높은 학업능력이 요구되므로 성적 외에도 다른 평가 요소들이 중요하게 작용할 수 있습니다.
+1. **성적**: 4등급은 좋은 성적이지만, 방사선학과의 경우 대체로 높은 등급을 요구하기 때문에 경쟁률이 매우 높을 가능성이 큽니다.
+2. **학생부 종합 평가**: 학생부 종합 평가는 단순히 성적뿐만 아니라 창의성, 활동성, 인성 등을 고려하므로 이 부분에서 좋은 점수를 받는 것이 중요합니다.
+3. **면접 및 실기**: 일부 학과에서는 면접이나 실기 시험을 통해 지원자의 적합성을 평가하기도 합니다.
+따라서, 정확한 답변을 위해서는 방사선학과의 모집요강과 최신 합격기준을 확인하시고, 성적 외에 다른 평가 요소들도 잘 준비하는 것이 좋습니다. 또한, 대학 입학 홈페이지나 입학처와 상담하여 자세한 정보를 얻는 것도 도움이 될 것입니다.
+만약 추가적인 조언이 필요하다면, 해당 학과의 모집요강을 확인하거나 동의대학교 입학처에 문의하시는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D344" t="n">
+        <v>0.06267825733952821</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>방사선학과의 최종등록자 데이터를 기준으로 보면, 방사선학과의 영어 등급 평균은 2.8이고, 수능 4개 영역 등급 평균은 3.82입니다. 
+따라서, 현재 정시 등급이 2.66이라면 이는 귀하의 성적이 평균보다 높음을 의미합니다. 따라서, 귀하는 방사선학과에 합격할 가능성이 있다고 볼 수 있습니다. 
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 방사선학과의 정시 모집에서 2.66이라는 GPA는 상대적으로 낮은 점수입니다. 방사선학과는 보통 과학적 사고력과 전문 지식이 필요하기 때문에, 이 분야에서는 높은 GPA가 선호됩니다.
+정확한 합격 확률을 예측하는 것은 어렵지만, 2.66이라는 점수로는 경쟁이 매우 치열할 수 있습니다. 특히 해당 모집단위의 모집인원과 지원자들의 평균 GPA를 고려해야 합니다.
+다음은 몇 가지 제안입니다:
+1. **추가 지원**: 다른 학과나 정시 모집군을 추가로 지원하는 것을 고려해보세요.
+2. **면접 준비**: 방사선학과는 면접 과정도 중요하게 평가하기 때문에, 면접 준비를 철저히 해보세요.
+3. **추천서 및 자기소개서**: 강력한 추천서나 독특한 자기소개서를 준비하여 지원자의 개인적 가치를 강조해보세요.
+결국, 최종 합격 여부는 여러 요인에 따라 결정되므로, 다양한 전략을 고려하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D345" t="n">
+        <v>0.1083300700055292</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>제공된 정보에 따르면, 경찰행정학과의 2024학년도 수능(일반학생전형) 최종등록자 평균 수능 4개 영역 등급은 4.12입니다. 귀하의 성적이 3.66이라면, 이는 평균보다 높은 성적입니다. 
+경쟁률이 2020년도에 비해 낮아졌다는 점도 긍정적인 요소로 작용할 수 있습니다. 경쟁률이 낮아지면 합격 가능성이 상대적으로 높아질 수 있기 때문입니다.
+따라서, 귀하의 성적이 평균보다 높고 경쟁률이 낮아진 점을 고려할 때, 희망을 가져도 될 것으로 보입니다. 다만, 최종 결과는 여러 변수에 따라 달라질 수 있으므로, 최선을 다해 준비하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>3.66이라는 성적은 일반적으로 경찰행정학과의 경우 좋은 점수일 것입니다. 그러나 정확한 합격 가능성 판단을 위해서는 다음과 같은 요소들을 고려해야 합니다:
+1. **전형 방식**: 농어촌학생전형의 경우, 수능성적이 아닌 다른 평가 기준이 주로 적용됩니다. 일반적으로 학생부 교과 성적, 지역 거주 경력 등이 중요하게 작용합니다.
+2. **학업역량 및 전공적합성**: 농어촌학생전형에서는 지원자의 학업 역량과 전공 적합성을 중점적으로 평가합니다. 따라서 수능 점수보다는 학생부 교과 성적이 더 중요할 수 있습니다.
+3. **지역 거주 경력**: 농어촌학생전형의 경우, 지원자가 농어촌 지역에서 거주한 경력을 요구하기 때문에 이 부분이 중요한 역할을 합니다.
+4. **모집인원 및 지원자 수**: 각 모집단위별로 정해진 합격 인원과 지원자의 수에 따라 합격 가능성은 달라질 수 있습니다.
+5. **기타 평가 요소**: 면접 성적, 추천서 등 기타 평가 요소도 고려됩니다.
+따라서 3.66이라는 점수만으로는 정확한 판단이 어렵습니다. 지원자의 학생부 교과 성적, 농어촌 거주 경력, 그리고 다른 평가 요소들을 종합적으로 고려해야 합니다. 
+추천 드리는 것은:
+- **학생부 교과 성적 확인**: 지원자가 높은 점수를 받았는지 확인하세요.
+- **농어촌 거주 경력 확인**: 이 부분이 충족되었는지 다시 한번 확인해 보세요.
+- **모집인원 및 지원자 수 조사**: 해당 전공의 모집인원과 지원자의 수를 파악하여 합격 가능성을 판단해 보세요.
+만약 위 요소들이 모두 충족된다면, 합격 가능성은 높아질 것입니다. 그러나 정확한 판단을 위해서는 동의대학교 입학처에 직접 문의하는 것이 가장 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D346" t="n">
+        <v>0.07591967963229232</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>귀하께서 지원하신 학과에 따라서 합격될 확률은 달라질 수 있습니다.
+2024년 동의대학교 일반학생전형에서 예비 25번 이상이 합격한 학과는 다음과 같습니다.
+- **영어영문학과**
+- **경영정보학과**
+- **e비즈니스학과**
+- **간호학과**
+- **신소재공학과**
+- **고분자나노공학과**
+- **의생명공학과**
+- **바이오의약공학과**
+- **식품공학과**
+- **산업경영빅데이터공학과**
+귀하께서 지원하신 학과가 위 학과에 포함된다면, 귀하께서 합격하실 확률은 있다고 볼 수 있습니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>25위 예비 합격자로서의 붙는 확률은 매우 낮지만, 완전히 배제할 수는 없습니다. 정시 모집인원에 미달한 경우에는 추가모집이 이루어질 수 있으며, 이때 예비합격자들이 우선적으로 선발될 가능성이 있습니다.
+다음과 같은 요소들을 고려해볼 필요가 있습니다:
+1. **모집인원**: 현재의 모집인원과 예비 합격자의 수를 비교하여 전체 경쟁률을 파악합니다.
+2. **기타 지원자들의 성적**: 다른 지원자들의 성적이 얼마나 높은지 확인해야 합니다.
+3. **추가모집 가능성**: 정시 모집이 미달된 경우 추가모집이 이루어질 가능성을 고려합니다.
+예비 합격자는 최소한의 기회를 가지고 있으므로, 등록금 납부 등의 절차를 철저히 따르고, 필요하다면 학교에 직접 문의하여 추가 정보를 얻는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D347" t="n">
+        <v>0.2071187077326167</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>동의대학교 정시 모집 전형에는 법경찰행정학부라는 학부는 존재하지않습니다.  
+동의대학교 경찰행정학과의 최종등록자와 최초합격자의 평균 성적을 비교하여 안정권과 문 닫고 들어갈 수 있는 성적을 추정할 수 있습니다.
+- **최종등록자 평균 성적:**
+   - 국어 + 수학 + 탐구(2개) 표준 변환 점수 합: 332.86
+   - 영어 등급: 4.00
+   - 수능 4개 영역 등급: 4.12
+   - 수능 4개 영역 표준 변환 점수 합: 447.86
+- **최초합격자 평균 성적:**
+  - 국어 + 수학 + 탐구(2개) 표준 변환 점수 합: 330.71
+  - 영어 등급: 3.14
+  - 수능 4개 영역 등급: 3.87
+  - 수능 4개 영역 표준 변환 점수 합: 452.57
+### 안정권과 문 닫고 들어갈 수 있는 성적 추정
+- **경찰행정학과:**
+  - 안정권: 최초합격자 평균 성적에 근접한 성적 (국어 + 수학 + 탐구(2개) 표준 변환 점수 합 약 331점 이상, 수능 4개 영역 표준 변환 점수 합 약 453점 이상)
+  - 문 닫고 들어갈 수 있는 성적: 최종등록자 평균 성적에 근접한 성적 (국어 + 수학 + 탐구(2개) 표준 변환 점수 합 약 333점 이상, 수능 4개 영역 표준 변환 점수 합 약 448점 이상)
+이 성적을 기준으로 준비하시면 안정권 또는 문 닫고 들어갈 수 있는 성적을 받을 수 있을 것입니다. 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 동의대학교 법경찰행정학부의 정시모집에서 안정적인 합격을 위해서는 다음과 같은 점수를 고려해야 합니다:
+1. **전년도 성적 분석**: 최근 몇 년간의 입학성적을 참고하면 가장 좋은 가늠자가 됩니다. 예를 들어, 2023년에 법경찰행정학부에서 안정적으로 합격한 학생들의 평균 수능 점수를 확인할 수 있습니다.
+2. **등급 분석**: 전년도 입학생들의 등급을 분석하여 대략적인 등급 범위를 파악합니다. 예를 들어, 90% 이상의 합격률을 보였다면, 해당 등급에 가까운 점수를 받는 것이 안정적입니다.
+3. **전형별 성적**: 동의대학교는 다양한 전형으로 모집하므로, 정시모집에서 요구하는 수능 최저등급을 확인해야 합니다. 이는 대략 4개 과목(국어, 영어, 수학, 사회) 중 2개 이상이 B등급 이상이어야 한다는 등의 조건일 수 있습니다.
+4. **추세 분석**: 최근 몇 년간의 입학성적 추세를 살펴보면, 평균적인 성적이 어느 정도였는지 파악할 수 있습니다. 이는 일반적으로 안정적인 합격을 위해서는 해당 추세보다 약간 높은 점수를 받는 것이 좋습니다.
+5. **경쟁률**: 법경찰행정학부의 경쟁률을 고려하여, 경쟁률이 높다면 더 높은 성적을 준비해야 합니다.
+6. **추천 전형**: 학생부종합전형 등 다른 전형에서도 안정적으로 합격할 수 있는 경우, 정시모집에서는 조금 낮은 점수를 받더라도 안정적인 합격이 가능합니다.
+일반적으로 동의대학교 법경찰행정학부에서 정시로 안정적으로 합격하기 위해서는 **수능 4개 과목 중 2개 이상 B등급** 이상을 받고, **전년도 입학생들의 평균 등급보다 약간 높은 점수**를 목표로 설정하는 것이 좋습니다. 예를 들어, 전년도에 A+와 B+를 받았다면, 올해는 최소 A+와 B+를 받고, 가능하다면 A+와 A를 받는 것이 안정적입니다.
+최종적으로 가장 정확한 정보는 동의대학교 입학처 홈페이지나 학부모포털을 통해 확인하는 것이 좋습니다. 또한, 입학사정관들이 직접 설명하는 세미나나 설명회에도 참석하여 최신 정보와 전형별 요구사항을 파악하는 것도 도움이 될 것입니다.</t>
+        </is>
+      </c>
+      <c r="D348" t="n">
+        <v>0.2133944443239984</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>24학년도 모집단위에서 보육가정상담학과에서 아동학과로 변경되었습니다. 아동학과에 대해서 대답을 해드리겠습니다.
+	아동학과의 최종등록자 데이터를 기준으로 보면, 아동학과의 영어 등급 평균은 6.33이고, 수능 4개 영역 등급 평균은 7.08입니다. 
+	따라서, 현재 정시 등급이 5.33라면 아동학과의 평균 등급보다 높은 성적을 가지고 있어 합격 가능성이 높습니다.
+	자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>5.33이라는 등급을 가지고 동의대학교 보육가정상담학과에 합격할 수 있는지는 여러 요소를 고려해야 합니다.
+1. **모집단위와 모집인원**: 먼저, 보육가정상담학과의 정원외 모집인원이 얼마나 되는지 확인해야 합니다. 표에서 보육가정상담학과는 인문사회과학대학 아동학과로 분류되어 있으며, 최대 13명까지 모집할 수 있습니다.
+2. **등급 평균**: 표에 나와 있는 합격자들의 등급 평균을 확인해야 합니다. 예를 들어, 아동학과의 경우 4.57이라는 평균 등급이 나와 있습니다. 이는 현재까지의 합격자들의 등급 평균입니다.
+3. **등급 상위자 선발**: 동점자 처리 기준에 따르면, 국어, 수학, 영어, 한국사, 사회(역사/도덕 포함), 과학교과 전 과목 등급 평균 상위자가 우선적으로 선발됩니다. 따라서 5.33이라는 등급이 해당 학과의 등급 평균보다 높다면 더 좋은 위치에 있을 수 있습니다.
+4. **동점자 처리**: 동점자가 발생할 경우, 등급 평균이 높은 순으로 선발되므로 5.33이라는 등급이 상위권에 속해 있다면 합격 가능성은 있습니다.
+따라서, 현재까지의 합격자들의 등급 평균을 확인하고, 자신의 등급이 해당 평균보다 높다면 합격 가능성이 있습니다. 하지만 최종 결정은 입학관리팀에서 이루어지므로, 정확한 정보를 얻기 위해서는 동의대학교 입학관리 홈페이지나 관계자에게 문의하는 것이 좋습니다.
+추가적으로, 지원자의 전반적인 성적과 학교생활기록부 등 기타 평가 요소도 고려되어 결정이 이루어지므로, 모든 자료를 잘 준비하고 제출하는 것이 중요합니다.</t>
+        </is>
+      </c>
+      <c r="D349" t="n">
+        <v>0.07477335629832092</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>동의대학교의 충원 합격자 발표 및 등록 일정에 따르면, 충원 합격자 발표는 1차, 2차, 그리고 3차 이후로 나뉘어 진행됩니다. 3차 이후의 충원 합격자 발표는 2024년 2월 15일(목) 19:00부터 2024년 2월 20일(화) 18:00까지 개별 전화 통보로 이루어집니다.
+예비 12번을 받으셨다면, 앞선 예비 번호를 받은 지원자들이 등록을 포기하거나 다른 대학에 등록하는 경우, 합격 가능성이 있습니다. 충원 합격은 지원자들의 등록 포기 여부에 따라 달라지므로, 정확한 예측은 어렵습니다. 하지만 예비 번호가 12번이라면, 충원 합격 가능성이 아예 없는 것은 아닙니다.
+충원 합격자 발표 기간 동안 전화 통보를 기다리시고, 다른 대학의 등록 상황도 주시하시기 바랍니다. 간절한 마음이 잘 전달되어 좋은 결과가 있기를 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교의 수능(일반학생전형) 최초합격자 및 충원합격자의 발표 일정과 기준을 보면, 다음과 같은 점들을 고려해야 합니다:
+1. **3차 충원 합격자 발표**: 2024년 2월 15일(목)부터 2024년 2월 20일(화)까지입니다.
+2. **동점자 처리 기준**:
+   - 1위: 면접고사 성적 상위자
+   - 2위: 서류평가 공동체역량 영역 성적 상위자
+   - 3위: 서류평가 전공적합성 영역 성적 상위자
+   - 4위: 교과 성적 상위자
+3. **결원 처리**: 결원 발생 시 예비후보 순위에 따라 충원 합격자를 선발합니다.
+4. **출결 기준**:
+   - 0~2일: 120점
+   - 3~6일: 90점
+   - 7~12일: 60점
+   - 13~20일: 30점
+   - 21일 이상: 0점
+5. **출결 기준 미달 시**: 충원 합격이 되었으나 등록 의사가 없는 경우 등록 포기자로 간주됩니다.
+**합격 가능성 평가**:
+- **예비 12번**: 이는 예비후보 순위를 나타내며, 12번은 상대적으로 낮은 순위입니다.
+- **출결 기준**: 출결이 7일 이상인 경우 점수가 크게 감소하므로, 이 부분에서 불리한 점이 있습니다.
+**추천 사항**:
+1. **면접 준비**: 면접고사 성적 상위자로 선발될 가능성을 높이기 위해 충분히 준비해야 합니다.
+2. **서류 제출**: 서류평가에서도 공동체역량과 전공적합성 영역에서 우수한 점수를 받도록 노력해야 합니다.
+3. **출결 확인**: 7일 이상의 결석은 피하고, 최대한 출석을 유지하는 것이 중요합니다.
+따라서 예비 12번이지만 충분히 준비와 노력하면 합격 가능성은 있습니다. 하지만 경쟁률이 높아서 확실하게 보장되는 것은 아닙니다.</t>
+        </is>
+      </c>
+      <c r="D350" t="n">
+        <v>0.1669991345273708</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>정시 성적 4.75로 지원 가능한 학과를 알아보겠습니다. 제공된 데이터에서 최종등록자의 수능 4개 영역 등급 평균을 기준으로 분석해보겠습니다.
+### 지원 가능 학과
+- **국어국문학과**: 4.92 (평균)
+- **중어중국학과**: 5.68 (평균)
+- **일본학과**: 4.87 (평균)
+- **영어영문학과**: 5.16 (평균)
+- **문헌정보학과**: 4.82 (평균)
+- **평생교육·청소년상담학과**: 5.22 (평균)
+- **아동학과**: 7.08 (평균)
+- **금융경영학과**: 5.41 (평균)
+- **재무부동산학과**: 5.82 (평균)
+- **무역학과**: 5.18 (평균)
+- **유통물류학과**: 5.45 (평균)
+- **회계학과**: 4.99 (평균)
+- **국제관광경영학과**: 5.41 (평균)
+- **호텔·컨벤션경영학과**: 6.12 (평균)
+- **외식경영학과**: 4.91 (평균)
+- **의료경영학과**: 5.92 (평균)
+- **식품영양학과**: 5.92 (평균)
+- **기계공학과, 로봇자동화공학과, 자동차공학과**: 6.30 (평균)
+- **조선해양공학과**: 6.16 (평균)
+- **신소재공학과, 고분자나노공학과**: 5.78 (평균)
+- **환경공학과, 화학공학과, 응용화학과**: 5.73 (평균)
+- **의생명공학과, 바이오의약공학과, 식품공학과**: 5.41 (평균)
+- **인간공학과, 제품디자인공학과**: 5.72 (평균)
+- **산업경영빅데이터공학과**: 5.27 (평균)
+- **인공지능학과**: 5.25 (평균)
+- **전기공학과, 전자공학과**: 5.37 (평균)
+- **게임공학과**: 4.78 (평균)
+- **영화학과**: 5.04 (평균)
+### 유아교육학과
+유아교육학과의 경우, 최종등록자의 수능 4개 영역 등급 평균이 4.18로 나타나 있습니다. 따라서, 4.75의 성적으로는 유아교육학과에 지원하기 어려울 것으로 보입니다.
+추가적인 정보나 문의사항이 있으시면 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>4.75의 등급점수를 얻으려면 수능 영어시험에서 높은 점수를 받아야 합니다. 수능 영어의 등급이 8등급 이상이어야 4.75의 등급점수가 나옵니다.
+유아교육학과에 지원할 때, 수능 영어 성적이 중요하지만, 학교생활기록부와 면접 등의 서류평가와 면접에서도 좋은 평가를 받는 것이 중요합니다. 따라서 다음과 같은 점들을 고려해보세요:
+1. **수능 영어 성적**: 8등급 이상을 목표로 해야 합니다.
+2. **학교생활기록부**: 학업역량과 전공적합성을 보여줄 수 있는 활동이나 경험을 기재해야 합니다.
+3. **면접**: 지원 동기와 학업계획, 그리고 유아교육에 대한 이해도를 잘 표현해야 합니다.
+유아교육학과는 교육 분야에서의 실무 경험이나 관련 활동이 중요하게 평가되므로, 이러한 경험을 강조하는 것이 도움이 될 수 있습니다. 또한, 학교생활기록부와 면접에서도 유아교육에 대한 열정과 적합성을 잘 보여줄 수 있어야 합니다.
+결론적으로 4.75의 등급점수만으로는 어렵게 느껴질 수 있지만, 다른 평가 요소들을 잘 준비한다면 가능성이 있습니다.</t>
+        </is>
+      </c>
+      <c r="D351" t="n">
+        <v>0.1340972317982231</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>보육가정상담학과의 최종등록자 데이터를 기준으로 보면, 아동학과의 영어 등급 평균은 6.33이고, 수능 4개 영역 등급 평균은 7.08입니다. 
+따라서, 현재 정시 등급이 4.16라면 아동학과의 평균 등급보다 높은 성적을 가지고 있어 합격 가능성이 높습니다. 즉, 추가합격까지 생각해서 합격할 가능성이 높습니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 정시 모집에서 보육가정상담학과(아동학과)로 지원하실 경우, 수능 성적과 교과성적이 중요합니다. 주요 정보를 바탕으로 답변 드리겠습니다:
+1. **수능 성적**: 
+   - 4.16등급은 상당히 좋은 점수입니다.
+   - 경쟁률이 높을 수 있으나, 최근 몇 년간의 경쟁률과 지원 인원 등을 고려하면 합격 가능성은 있습니다.
+2. **교과성적**:
+   - 교과성적 반영방법에 따라 8과목 또는 12과목 중 상위 등급을 선택하여 반영합니다.
+   - 보육가정상담학과는 인문사회과학 분야이므로, 국어, 수학, 영어 등의 성적이 중요합니다.
+3. **경쟁률**:
+   - 최근 몇 년간의 경쟁률을 확인해야 합니다. 예를 들어 2023년 보육가정상담학과의 경쟁률은 약 17:1이었습니다.
+   - 지원 인원도 고려해야 하며, 이 학과는 일반적으로 지원자가 많습니다.
+4. **추합**:
+   - 추합 점수를 확인하여 합격 가능성을 판단할 수 있습니다. 추합 점수가 충분히 높다면 합격 가능성은 높아집니다.
+   - 예를 들어, 추합 점수가 300점 이상이면 합격 가능성이 높습니다.
+5. **추천**:
+   - 최종적으로는 모집단위별로 정확한 추합 점수와 경쟁률을 확인해야 합니다.
+   - 입학사정관제를 통해 추가 지원 자료를 제출하여 학교의 특성에 맞게 지원하는 것이 좋습니다.
+결론적으로, 4.16등급은 좋은 성적입니다만, 최종 합격 여부는 경쟁률과 지원 인원, 추합 점수 등 다양한 요인에 따라 결정됩니다. 정확한 정보를 얻기 위해서는 동의대학교 입학처 웹사이트나 전화로 문의하시는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D352" t="n">
+        <v>0.03505299299986672</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>아니요. 소프트웨어융합학과는 정시로 지원할 수 없습니다.</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>2024년 현재, 소프트웨어융합학과는 정시 모집에 포함되어 있지 않습니다. 따라서 정시로 지원하는 것은 불가능합니다.
+소프트웨어융합학과는 주로 수시모집에서 선발되며, 특히 나군 학생부종합전형이나 실기/실적 위주 전형에서 많은 지원자가 있습니다. 이들 전형에서는 평균적으로 다음과 같은 등급을 받은 학생들이 입학에 성공하고 있습니다:
+1. **나군 학생부종합전형**:
+   - 국어: 4등급 이상
+   - 수학: 3등급 이상 (특히 수학(확률과통계)이나 수학(미적분/기하)에서 높은 점수를 받는 것이 중요)
+   - 영어: 5등급 이상
+2. **실기/실적 위주 전형**:
+   - 실기나 실적 부분에서 우수한 성과를 보여줘야 합니다.
+따라서 정시로 지원하려면 해당 학과가 정시 모집에 포함되어 있어야 하며, 현재로서는 소프트웨어융합학과는 정시 모집 대상이 아닙니다. 
+더 자세한 정보나 변경 사항은 공식 입학 홈페이지 (https://ipsi.deu.ac.kr/main.do)를 참조하시거나 학교 관계자에게 문의하시는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D353" t="n">
+        <v>1.07620448149537e-07</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>소프트웨어융합학과는 서류 평가(공동체 역량, 학업 역량, 전공 적합성)과 면접 고사(400점 만점), 
+	학생부 교과성적을 합쳐서 평가합니다. 
+	준비해야하는 서류와 자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>『소프트웨어융합학과』의 경우, 면접 점수와 서류 평가의 비중이 동일하게 60%와 40%로 설정되어 있습니다. 따라서 면접뿐만 아니라 서류 평가에서도 중요한 역할을 합니다.
+서류 준비에 있어서 주요한 내용은 다음과 같습니다:
+1. **고교 학생부 온라인 제공 동의**: 고교 졸업(예정)자는 이 부분을 제출하지 않아도 됩니다.
+2. **학교생활기록부 대체 서류 (선택적 제출)**: 검정고시 출신자와 외국고교 졸업 예정자는 선택적으로 학교생활기록부 대체 서류를 제출할 수 있습니다.
+특히, 면접에서 요구되는 내용과 관련하여서는:
+- **지원동기 및 학업계획**: 지원 동기를 설명하고, 입학 후 어떤 학업 계획을 가지고 있는지 구체적으로 이야기해야 합니다.
+- **학업역량**: 고교 생활 중 학업에 대한 어려움과 이를 극복하기 위해 한 노력을 이야기해야 합니다.
+- **전공적합성**: 지원한 전공(계열)과 관련된 교내 활동을 설명해야 합니다.
+따라서, 서류 준비 시에는 면접에서 요구되는 내용과 일치하는 서류를 체크리스트 형태로 만들어 준비하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D354" t="n">
+        <v>0.02496286427715115</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>동의대학교 소프트웨어공학부의 2024학년도 수능(일반학생전형) 최초합격자의 수능 4개 영역 등급 평균은 4.12입니다. 따라서, 4.08의 성적은 최초합격자의 평균 등급보다 약간 높은 수준입니다. 
+	최초합격자의 평균 등급과 비교적 근접한 성적이므로, 최초합격 가능성은 있지만 확실하지는 않습니다. 추가적인 요소나 경쟁률에 따라 결과가 달라질 수 있습니다. 
+	정확한 정보는 동의대학교 입학처에 문의하는 것이 좋습니다. 추가적인 문의는 "https://ipsi.deu.ac.kr/main.do"에서 확인할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 소프트웨어공학부의 경우, 수능 최종 등록자의 평균 점수와 경쟁률을 고려해보겠습니다.
+- **소프트웨어공학부**:
+  - 모집인원: 120명
+  - 지원인원: 45명 (최초합격자 포함)
+  - 경쟁률: 약 3.33 : 1 (45 / 120)
+  - 평균 수능 점수: 446.69
+현재 질문자의 수능 성적이 4.08로, 이는 표준점수로 보겠습니다. 4.08의 표준점수가 실제 점수로 환산되면 대략 450점 정도가 됩니다.
+- **최근 평균 수능 점수**:
+  - 2023년도 동의대학교 소프트웨어공학부의 최종 합격자들의 평균 수능 점수가 약 446.69점으로, 질문자의 점수가 이보다 약간 높습니다.
+- **경쟁률**:
+  - 현재 모집인원 대비 지원자가 적어 경쟁률이 낮은 편입니다.
+따라서, 질문자의 수능 성적 4.08 (약 450점)는 소프트웨어공학부의 최초합격자로 충분히 가능할 것으로 보입니다.
+하지만 정확한 확률을 판단하기 위해서는:
+1. 최근 몇 년간의 수능 성적 분포를 확인해야 합니다.
+2. 지원자의 전체 성적 분포와 경쟁률을 고려해야 합니다.
+따라서, 질문자가 최초합격자로 선발될 가능성이 높지만, 확실한 것은 아니므로 추가 정보 수집과 준비가 필요합니다.</t>
+        </is>
+      </c>
+      <c r="D355" t="n">
+        <v>0.1418854706458846</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>소프트웨어융합학과의 정시 모집에 대한 구체적인 합격 등급 정보는 제공된 Context에 포함되어 있지 않습니다. 소프트웨어융합학과는 나군 학생부종합(조기취업형계약학과전형)으로도 모집하며, 이 경우 서류 60%와 면접 40%의 비율로 전형요소를 반영합니다.
+정확한 합격 가능성을 확인하기 위해서는 해당 학과의 최근 합격자 평균 등급이나 입시 결과를 참고해야 합니다. 이러한 정보는 대학의 입학처 홈페이지나 모집요강에서 확인할 수 있습니다. 추가적인 정보가 필요하다면 "https://ipsi.deu.ac.kr/main.do"를 방문하여 문의하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 제공된 정보로는 "소프트웨어융합학과"에 대한 정시 모집단위 및 모집인원이 직접적으로 나와 있지 않습니다. 그러나 "소프트웨어공학부"에 대한 정보가 있습니다.
+"소프트웨어공학부"의 경우, 정원외 지원자격에서 최대선발 가능인원으로 45명을 제시하고 있으며, 정시 모집군 변경에서도 "소프트웨어공학부(컴퓨터소프트웨어공학, 응용소프트웨어공학)"로 명시되어 있습니다.
+"소프트웨어융합학과"가 "소프트웨어공학부"의 일부로 분류되는지 확인하기 위해서는 추가적인 정보가 필요합니다. 
+만약 "소프트웨어융합학과"가 "소프트웨어공학부"의 하위 학과로 분류되어 있다면, 5등급으로 지원 가능할 수 있습니다. 하지만 만약 독립된 학과라면, 해당 학과에 대한 정보를 확인해야 합니다.
+추가적으로, 정시 모집군 변경이나 전형 요소 반영비율 등에 대한 정보도 필요합니다. 
+만약 "소프트웨어융합학과"가 독립된 학과로 분류되어 있다면, 해당 학과의 최저 합격 기준을 확인해야 합니다. 제공된 데이터에서 정확한 정보를 찾지 못했으므로, 공식 홈페이지 (https://ipsi.deu.ac.kr/main.do)를 참조하거나 관계자에게 문의하는 것이 가장 확실합니다.</t>
+        </is>
+      </c>
+      <c r="D356" t="n">
+        <v>0.2433035393170419</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>정확한 답변을 위해서는 더 많은 정보가 필요하지만, 제공된 데이터를 바탕으로 대략적인 판단을 할 수 있습니다.
+### 신소재공학과, 분자나노공학과 (공과대학) - 2024학년도
+- **최초합격자 평균 수능 4개 영역 등급**: 5.32
+- **최종등록자 평균 수능 4개 영역 등급**: 5.78
+### 귀하의 성적
+- **수능 4개 영역 등급**: 4.28
+귀하의 성적이 신소재공학과의 최초합격자와 최종등록자의 평균 등급보다 높습니다. 따라서, 동의대학교 신소재공학과에 합격할 가능성이 높다고 판단됩니다. 
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>4.28이라는 성적을 가지고 동의대학교 신소재공학과에 진학하기는 어렵다고 볼 수 있습니다.
+신소재공학과의 지원자들의 평균 성적이 다음과 같습니다:
+- 한의예과(수학&lt;미적분/기하&gt;): 1.00
+- 한의예과(수학&lt;확률과통계&gt;): 1.00
+- 공과대학 신소재공학과, 분자나노공학과: 4.33
+이 중에서 가장 가까운 수준은 4.33입니다. 이는 평균 성적이 4.28보다 약간 높습니다.
+다음은 고려해야 할 몇 가지 요소들입니다:
+1. **경쟁률**: 신소재공학과의 경쟁률이 1.45로 상대적으로 낮지 않으므로, 성적이 조금 더 높다면 충원 합격 가능성은 있습니다.
+2. **가산점**: 수능 외에 가산점을 받을 수 있는 기회가 있다면 이 점수를 활용할 수 있습니다.
+3. **추천서 및 자기소개서 등 서류 평가**: 전형요소 반영비율이 70%는 서류평가와 면접이 중요하므로, 강력한 추천서나 자기소개서 등을 준비한다면 도움이 될 수 있습니다.
+4. **면접 성적**: 면접에서도 좋은 점수를 받을 경우 합격 가능성은 높아질 것입니다.
+결론적으로 4.28의 성적만으로는 신소재공학과에 진학하기 어렵다고 판단되지만, 다른 요인들을 잘 활용한다면 충원 합격 가능성은 있습니다. 자세한 정보를 얻기 위해서는 동의대학교 입학처 웹사이트나 전화로 문의하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D357" t="n">
+        <v>0.1828859218475924</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>아니요. 수능 일반학생전형은 자기소개서가 필요없습니다.</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 수능(일반학생전형)에서는 자기소개서가 필수적으로 요구되는 것은 아닙니다. 이 전형은 주로 수능 점수를 기준으로 학생들을 선발합니다. 그러나 일부 모집단위에서는 자기소개서를 선택적으로 요구할 수도 있으므로, 해당 모집단위의 세부 안내를 확인해보시는 것이 좋습니다.
+만약 자기소개서가 필요하다면, 다음과 같은 내용을 포함하는 것이 도움이 될 수 있습니다:
+1. 개인적 특성과 강점
+2. 학업 목표와 계획
+3. 관련 경험 및 활동
+4. 미래의 꿈과 비전
+하지만 기본적으로는 수능 점수만으로 지원할 수 있으므로, 해당 모집단위의 공고를 체크하여 자세한 요구 사항을 확인하시기 바랍니다.
+더 궁금하신 점이 있으면 https://ipsi.deu.ac.kr/main.do 웹사이트를 참조하거나 입학처에 문의해보세요.</t>
+        </is>
+      </c>
+      <c r="D358" t="n">
+        <v>4.777004755026353e-06</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>동의대학교의 수능 정시 모집에서 합격 가능성을 평가하기 위해서는 각 학과의 평균 등급과 표준 편차를 참고하는 것이 중요합니다. 제공된 데이터에 따르면, 각 학과의 수능 4개 영역 등급 평균과 표준 편차가 나와 있습니다. 
+예를 들어, 인문사회과학대학의 국어국문학과의 경우, 최초 합격자의 수능 4개 영역 등급 평균은 4.65이고, 최종 등록자의 경우 4.92입니다. 
+따라서, 수능 4개 영역 등급이 4.5라면, 일부 학과에서는 합격 가능성이 있을 수 있습니다. 그러나, 각 학과마다 요구하는 등급이 다르므로, 지원하고자 하는 학과의 평균 등급과 비교해보는 것이 중요합니다.
+추가 모집의 경우, 경쟁률이 낮아질 수 있으므로 합격 가능성이 높아질 수 있습니다. 하지만, 추가 모집에 대한 정보는 학교의 공식 홈페이지나 입학처에 문의하는 것이 가장 정확합니다.
+자세한 사항은 동의대학교 입학처에 문의하시기 바랍니다. 추가 정보는 "https://ipsi.deu.ac.kr/main.do"에서 확인할 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>4.5라는 점수만으로는 확실한 답변을 드리기 어렵습니다. 추가 모집 가능성은 다음과 같은 요인들에 따라 달라질 수 있습니다:
+1. **모집 인원과 지원자 수**: 각 모집단위의 정원과 실제 지원자의 수가 중요합니다.
+2. **성적 순위**: 4.5라는 점수는 전체 지원자 중에서 어느 위치에 있는지 확인해야 합니다.
+3. **전형 방식**: 정시 일반학생전형, 실기/실적(경기실적우수자전형), 학생부교과, 학생부종합 등 다양한 전형이 있으므로 해당 전형의 성적 반영 방법을 확인해야 합니다.
+4. **동점자 처리 기준**: 동점자가 발생할 경우 어떻게 처리되는지 확인해야 합니다.
+5. **추가 모집 가능성**: 정시에서 미충원된 인원이 추가모집으로 이월될 가능성이 있습니다.
+6. **개인적 요소**: 면접 성적, 서류 평가 등 개인적인 요소도 고려됩니다.
+따라서, 가장 정확한 답변을 드리기 위해서는 동의대학교 입학처 웹사이트나 전화로 문의하시는 것이 좋습니다. 또한, 입학예정자 명단이나 동점자 처리 기준 등을 확인해보시면 더 구체적인 정보를 얻으실 수 있을 것입니다.
+추가적으로, [https://ipsi.deu.ac.kr/main.do](https://ipsi.deu.ac.kr/main.do) 웹사이트에서 최신 정보와 안내를 확인하실 수 있습니다.</t>
+        </is>
+      </c>
+      <c r="D359" t="n">
+        <v>0.3120144729551707</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>신소재학과의 최종등록자 데이터를 기준으로 보면, 신소재공학과의 영어 등급 평균은 5.06이고, 수능 4개 영역 등급 평균은 5.78입니다. 
+따라서, 신소재공학과의 평균 등급보다 높은 성적을 가지고 있으시면 합격 가능성이 올라갑니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>2023년 동의대학교 신소재공학과와 분자나노공학과의 모집요강을 바탕으로 추정해보겠습니다.
+신소재공학과와 분자나노공학과는 같은 학부이지만, 각각 다른 모집단위로 운영됩니다. 일반적으로 동의대학교 공과대학의 신소재공학과와 분자나노공학과는 B등급 내외에서 합격 가능성이 높습니다.
+2023년 동의대학교 공과대학의 일부 모집단위의 최저합격 기준을 보면:
+- **기계공학과, 로봇자동화공학과, 자동차공학과**: 0.87등급
+- **조선해양공학과**: 0.83등급
+- **신소재공학과, 분자나노공학과**: 1.45등급
+따라서 신소재공학과와 분자나노공학과의 경우 대략적으로 B등급(1.00) 이상이면 합격 가능성이 높습니다.
+하지만 정확한 등급은 매년 변동될 수 있으므로, 최신 모집요강을 확인하시거나, 동의대학교 입학처 웹사이트를 참조하시는 것이 가장 정확할 것입니다.</t>
+        </is>
+      </c>
+      <c r="D360" t="n">
+        <v>0.0882204882287677</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>작년 동의대학교 신소재공학과의 최종 등록자 평균 표준 변환 점수는 378.15점이었습니다. 따라서, 귀하의 표준점수 447점은 작년 신소재공학과의 평균 점수보다 훨씬 높습니다. 이 점수라면 신소재공학과에 합격할 가능성이 매우 높다고 할 수 있습니다. 
+추가적인 정보나 문의사항이 있으시면 "https://ipsi.deu.ac.kr/main.do"를 방문해 주시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 정시 모집에서 표준점수를 환산할 때, 작년 신소재공학과의 최종 평균 점수가 447점보다 약간 높았다면, 이는 몇 가지 요인으로 인해 가능성이 있습니다:
+1. **모집인원 및 지원자 수**: 작년에 신소재공학과의 모집인원이 늘어나거나 지원자가 줄었을 경우, 경쟁률이 상대적으로 낮아져 평균 점수가 높아질 수 있습니다.
+2. **지원자의 성적 분포**: 작년에는 고득점자들이 많았거나 저득점자들이 적게 지원했을 가능성이 있습니다. 이는 전체 평균 점수를 끌어올릴 수 있습니다.
+3. **면접 결과**: 일부 모집단위에서는 면접 점수가 포함되어 평균 점수를 결정합니다. 작년에는 면접에서 우수한 성적을 받은 지원자가 많았다면, 이로 인해 전체 평균 점수가 높아질 수 있습니다.
+4. **가산점**: 일부 모집단위에서는 가산점을 적용하여 최종 점수가 결정됩니다. 작년에는 많은 지원자가 가산점을 받았을 가능성이 있습니다.
+5. **학과 특성**: 신소재공학과는 일반적으로 높은 수능 점수를 요구하는 학과 중 하나입니다. 작년에는 이 학과에 대한 관심이 높아져 고득점자들이 많이 지원했을 수도 있습니다.
+따라서, 2024년에도 표준점수가 447점으로 환산될 가능성이 있지만, 작년의 상황과 비교하여 결정됩니다. 정확한 예측은 아직까지는 불가능하며, 최종 결과는 모집단위별 지원자 수와 경쟁률 등 다양한 요인에 따라 달라질 수 있습니다.
+만약 확실한 정보를 원하신다면, 동의대학교 입학처 웹사이트나 전화로 문의하시는 것이 가장 정확할 것입니다.</t>
+        </is>
+      </c>
+      <c r="D361" t="n">
+        <v>0.02924892379384652</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>동의대학교 신소재공학부(일반학생전형)의 최종등록자 데이터를 바탕으로 판단해보겠습니다.
+	신소재공학부의 최종등록자 평균 성적은 다음과 같습니다:
+	- 국어 + 수학 + 탐구(2개) (가산점 포함) 표준 변환 점수 합: 평균 271.64, 표준 편차 19.52
+	- 영어 등급: 평균 5.06, 표준 편차 1.22
+	- 수능 4개 영역 등급: 평균 5.78, 표준 편차 0.49
+	- 수능 4개 영역 (가산점 포함) 표준 변환 점수 합: 평균 378.15, 표준 편차 21.81
+	귀하의 성적이 4.1~4.2등급대라면, 신소재공학부의 최종등록자 평균 성적과 비교했을 때 다소 높은 편입니다. 특히, 영어 등급과 수능 4개 영역 등급에서 차이가 있을 수 있습니다.
+	따라서, 귀하의 성적이 신소재공학부의 최종등록자 평균 성적과 비교했을 때 다소 높으므로, 합격 가능성은 높습니다. 그러나, 최종 합격 여부는 지원자 전체의 성적 분포와 경쟁률에 따라 달라질 수 있습니다.
+	더 자세한 정보나 상담이 필요하다면, 동의대학교 입학처에 문의하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>4.3등급대의 성적이면 신소재공학부(신소재공학과, 고분자나노공학과)의 일반학생전형에서 합격 가능성은 낮지만, 아직 최종 결정이 내려지기 전까지는 모든 것이 가능합니다.
+신소재공학부의 경우 다음과 같은 점을 고려해야 합니다:
+1. **성적 기준**: 신소재공학과와 고분자나노공학과의 모집인원은 각각 26명입니다. 성적이 4.1~4.2등급대라면, 이는 상당히 높은 등급이며, 일반적으로 이런 등급을 가진 학생들은 대다수의 공과대학에서 합격할 수 있습니다.
+2. **전형 요소**: 나군 수능(일반학생전형)에서는 성적이 주요한 평가 기준이지만, 다른 요인들도 고려됩니다:
+   - **면접 성적**: 일부 모집단위에서는 면접 점수가 포함될 수 있습니다.
+   - **학업역량**: 학교생활기록부와 수능 성적을 종합적으로 평가합니다.
+3. **동점자 처리**: 동점자가 발생할 경우, 등급 평균이 결정적인 역할을 합니다. 4.1~4.2등급대라면, 이는 상당히 높은 점수로, 동점자 처리 시 유리한 위치에 있을 수 있습니다.
+4. **결원 선발**: 모집인원 미달 시 추가 모집이 가능합니다. 따라서, 현재의 성적만으로 판단하기보다는 전체적인 지원 경쟁률과 모집 상황을 고려해야 합니다.
+### 조언:
+1. **성적 확인**: 최종적으로 제출할 수 있는 성적을 다시 한 번 확인하세요.
+2. **면접 준비**: 면접 점수가 포함되는 경우, 충분히 준비해두세요.
+3. **전형 요소 종합**: 학교생활기록부와 수능 성적을 종합적으로 평가받는다는 점을 기억하십시오.
+결론적으로, 4.1~4.2등급대라면 신소재공학부에서 합격 가능성은 있지만, 확실한 것은 아닙니다. 최종 결정은 입학전형의 전체적인 경쟁률과 모집 상황에 따라 달라질 수 있으므로, 가능한 한 많은 정보를 수집하고 준비하는 것이 중요합니다.</t>
+        </is>
+      </c>
+      <c r="D362" t="n">
+        <v>0.2152577713141971</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>동의대학교 인공지능학과의 수능 일반학생전형 최초합격자 성적은 다음과 같습니다:
+- **모집 인원**: 15명
+- **지원 인원**: 24명
+- **경쟁률**: 1.60
+- **충원 합격 (후보순위)**: 5명
+- **국어 + 수학 + 탐구(2개) (가산점 포함) 표준 변환 점수 합**: 평균 301.87, 표준 편차 12.38
+- **영어 등급**: 평균 4.13, 표준 편차 0.71
+- **수능 4개 영역 등급**: 평균 4.98, 표준 편차 0.25
+- **수능 4개 영역 (가산점 포함) 표준 변환 점수 합**: 평균 415.80, 표준 편차 10.49
+이 성적을 참고하여 준비하시기 바랍니다. 추가적인 정보가 필요하면 "https://ipsi.deu.ac.kr/main.do"를 방문해 주세요.</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 인공지능학과의 나군(수능 일반학생전형) 최소 합격 기준 점수는 다음과 같습니다:
+- **국어**: 약 135점 (대략적인 추정치, 정확한 점수는 공식 발표를 확인해주세요)
+- **수학**: 약 90점 (대략적인 추정치, 정확한 점수는 공식 발표를 확인해주세요)
+- **영어**: 약 125점 (대략적인 추정치, 정확한 점수는 공식 발표를 확인해주세요)
+이러한 성적은 일반적으로 최소 합격 기준을 나타내지만, 실제 합격선은 모집인원과 지원자 수에 따라 변동될 수 있습니다. 따라서 가장 정확한 정보는 동의대학교 입학처 웹사이트나 공식 발표를 통해 확인하시기 바랍니다.
+또한, 인공지능학과는 실기/실적 요소가 포함된 전형이므로, 수능 성적이 최종 합격에 큰 영향을 미치지만, 다른 평가 항목들도 중요한 역할을 합니다.</t>
+        </is>
+      </c>
+      <c r="D363" t="n">
+        <v>0.3322422518601387</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>동의대학교의 정시 성적을 기준으로 5.27의 성적으로 충원 합격(추합)이 가능한지 확인하기 위해서는 각 학과의 최종 등록자 성적을 비교해보아야 합니다. 아래는 각 학과의 수능 4개 영역 등급 평균과 표준 편차를 기준으로 5.27 성적이 충원 합격 가능한지 확인한 결과입니다:
+1. **인문사회과학대학**
+   - 국어국문학과: 평균 4.92, 표준 편차 0.35
+   - 중어중국학과: 평균 5.68, 표준 편차 0.74
+   - 일본학과: 평균 4.87, 표준 편차 0.13
+   - 영어영문학과: 평균 5.16, 표준 편차 0.66
+   - 문헌정보학과: 평균 4.82, 표준 편차 0.33
+   - 평생교육·청소년상담학과: 평균 5.22, 표준 편차 0.29
+   - 아동학과: 평균 7.08, 표준 편차 0.56
+   - 유아교육과: 평균 4.18, 표준 편차 0.25
+   - 광고홍보학과: 평균 4.47, 표준 편차 0.18
+   - 미디어커뮤니케이션학과: 평균 4.29, 표준 편차 0.23
+   - 법학과: 평균 4.27, 표준 편차 0.27
+   - 경찰행정학과: 평균 4.12, 표준 편차 0.18
+   - 소방방재행정학과: 평균 4.43, 표준 편차 0.40
+   - 행정학과: 평균 4.36, 표준 편차 0.33
+   - 사회복지학과: 평균 4.69, 표준 편차 0.23
+2. **상경대학**
+   - 금융경영학과: 평균 5.41, 표준 편차 0.52
+   - 재무부동산학과: 평균 5.82, 표준 편차 1.25
+   - 무역학과: 평균 5.18, 표준 편차 0.50
+   - 유통물류학과: 평균 5.45, 표준 편차 0.52
+   - 경영학과: 평균 4.69, 표준 편차 0.22
+   - 회계학과: 평균 4.99, 표준 편차 0.41
+   - 경영정보학과: 평균 4.31, 표준 편차 0.23
+   - e비즈니스학과: 평균 4.53, 표준 편차 0.36
+   - 국제관광경영학과: 평균 5.41, 표준 편차 0.56
+   - 호텔·컨벤션경영학과: 평균 6.12, 표준 편차 0.77
+   - 외식경영학과: 평균 4.91, 표준 편차 0.28
+3. **의료보건생활대학**
+   - 간호학과: 평균 3.37, 표준 편차 0.29
+   - 임상병리학과: 평균 4.15, 표준 편차 0.12
+   - 치위생학과: 평균 4.18, 표준 편차 0.20
+   - 방사선학과: 평균 3.82, 표준 편차 0.20
+   - 의료경영학과: 평균 5.92, 표준 편차 1.08
+   - 물리치료학과: 평균 3.62, 표준 편차 0.15
+   - 식품영양학과: 평균 5.92, 표준 편차 1.06
+4. **한의과대학**
+   - 한의예과(수학&lt;미적분/기하&gt;): 평균 1.21, 표준 편차 0.09
+   - 한의예과(수학&lt;확률과통계&gt;): 평균 1.20, 표준 편차 0.05
+5. **공과대학**
+   - 기계공학과, 로봇자동화공학과, 자동차공학과: 평균 6.30, 표준 편차 1.1
+   - 조선해양공학과: 평균 6.16, 표준 편차 1.00
+   - 신소재공학과, 분자나노공학과: 평균 5.78, 표준 편차 0.49
+   - 건축학과(5년제), 건축공학과, 토목공학과, 도시공학과: 평균 4.69, 표준 편차 0.25
+   - 환경공학과, 화학공학과, 응용화학과: 평균 5.73, 표준 편차 0.57
+   - 의생명공학과, 바이오의약공학과, 식품공학과: 평균 5.41, 표준 편차 0.65
+   - 인간공학과, 제품디자인공학과: 평균 5.72, 표준 편차 0.73
+   - 산업경영빅데이터공학과: 평균 5.27, 표준 편차 0.43
+6. **ICT융합공과대학**
+   - 컴퓨터공학과: 평균 4.29, 표준 편차 0.16
+   - 소프트웨어공학부: 평균 4.49, 표준 편차 0.30
+   - 인공지능학과: 평균 5.25, 표준 편차 0.35
+   - 전기공학과, 전자공학과: 평균 5.37, 표준 편차 0.60
+   - 디지털콘텐츠학과: 평균 4.47, 표준 편차 0.24
+   - 게임공학과: 평균 4.78, 표준 편차 0.20
+   - 영화학과: 평균 5.04, 표준 편차 0.76
+7. **예술디자인체육대학**
+   - 패션디자인학과: 평균 4.46, 표준 편차 0.31
+위의 정보를 바탕으로, 5.27의 성적으로 충원 합격이 가능한 학과는 다음과 같습니다:
+- 인문사회과학대학: 중어중국학과, 영어영문학과, 평생교육·청소년상담학과, 아동학과
+- 상경대학: 금융경영학과, 재무부동산학과, 무역학과, 유통물류학과, 호텔·컨벤션경영학과, 외식경영학과
+- 의료보건생활대학: 의료경영학과, 식품영양학과
+- 공과대학: 기계공학과, 로봇자동화공학과, 자동차공학과, 조선해양공학과, 신소재공학과, 분자나노공학과, 환경공학과, 화학공학과, 응용화학과, 의생명공학과, 바이오의약공학과, 식품공학과, 인간공학과, 제품디자인공학과, 산업경영빅데이터공학과
+- ICT융합공과대학: 인공지능학과, 전기공학과, 전자공학과, 영화학과
+위 학과들은 5.27의 성적으로 충원 합격이 가능할 것으로 보입니다. 더 자세한 정보는 동의대학교 입학처에 문의하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>5.27이라는 점수를 보고 정확한 판단을 내리기 위해서는 몇 가지 정보가 필요합니다:
+1. 해당하는 모집군 (예: &lt;가&gt;군, &lt;나&gt;군 등)과 모집단위를 아시는지?
+2. 지원하고자 하는 모집단위의 최저 합격 기준 점수를 알고 계신지?
+일반적으로 동의대학교의 정시 모집에서는 수능 성적을 주요 평가 요소로 사용합니다. 하지만, 다른 평가 항목 (예: 학생부 교과성적, 면접 등)도 함께 고려되기 때문에 단순히 수능 점수만으로는 판단하기 어렵습니다.
+특정 모집단위의 최저합격 기준 점수를 확인하신 후, 해당 점수가 충족되면 가능할 것으로 보입니다. 하지만 정확한 답변을 위해서는 동의대학교 입학처 웹사이트나 전화로 문의하시는 것이 가장 좋습니다. 그곳에서는 각 모집단위별 최종 합격 기준 점수와 기타 평가 요소에 대한 자세한 정보를 제공해 줄 것입니다.
+추천되는 방법은:
+1. 동의대학교 입학처 웹사이트를 방문하여 해당 년도의 정시 모집요강을 확인합니다.
+2. 전화로 문의하거나, 온라인 상담을 이용하여 직접 확인하는 것입니다.</t>
+        </is>
+      </c>
+      <c r="D364" t="n">
+        <v>0.07067626658205818</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>소프트웨어공학부의 최종등록자 데이터를 기준으로 보면, 소프트웨어공학부의 영어 등급 평균은 3.77이고, 수능 4개 영역 등급 평균은 4.49입니다. 
+따라서, 현재 정시 등급이 4.2라면 소프트웨어공학부의 평균 등급보다 높은 성적을 가지고 있어 합격 가능성이 높습니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>4.2라는 점수는 중간 정도의 성적이므로, 소프트웨어공학부에 지원하는 데에는 가능성이 있지만 확률은 낮을 수 있습니다.
+소프트웨어공학부는 일반적으로 높은 경쟁률을 보이는 학과로, 특히 정시 모집에서는 고득점자들이 많이 선발됩니다. 그러나 4.2의 성적도 일부 모집단위에서 합격할 수 있는 기회가 있을 수 있습니다.
+다음 사항들을 참고하시면 도움이 될 것입니다:
+1. **모집인원과 경쟁률**: 소프트웨어공학부의 정시 모집인원을 확인하고, 현재 지원자의 수와 경쟁률을 파악하세요.
+2. **전형요소 반영비율**: 대부분의 전형에서는 수능 성적이 주요 평가 요소입니다. 4.2라는 점수는 중간 정도이므로, 다른 평가 요소들(면접 등)에서 좋은 성적을 보여야 합니다.
+3. **면접 준비**: 면접에서도 좋은 성적을 보여주어야 합니다. 지원동기와 학업계획, 전공적합성 등을 잘 준비해야 합니다.
+결론적으로 4.2의 점수로 소프트웨어공학부에 합격하는 것은 가능하지만, 경쟁률이 높아서 확실한 보장은 없습니다. 다른 평가 요소들에서 좋은 성적을 보여주고, 면접에서도 잘 준비해야 합니다.</t>
+        </is>
+      </c>
+      <c r="D365" t="n">
+        <v>0.07624280546884782</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>화학환경공학부의 최종등록자 데이터를 기준으로 보면, 화학환경공학부의 영어 등급 평균은 4.82이고, 수능 4개 영역 등급 평균은 5.73입니다. 
+따라서, 현재 정시 등급이 3.92라면 화학환경공학부의 평균 등급보다 높은 성적을 가지고 있어 합격 가능성이 높습니다. 즉, 추가합격까지 생각해서 합격할 가능성이 높습니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>为了判断您能否被 화학환경공학부 (化学环境工程学部) 录取，我们需要考虑以下几个因素：
+1. **最低录取分数线**：不同专业和学院有不同的录取分数线。请确认该专业的具体分数线是多少。
+2. **您的成绩**：您提到的3.92是您的平均分吗？如果是的话，请提供具体的科目分数分布情况，以便更准确地评估。
+3. **其他要求**：除了学术成绩外，某些专业可能还有额外的要求，如面试、特长等。请确认该专业是否有这些附加条件。
+4. **招生计划和名额**：查看该专业的具体招生人数以及是否已经招满。
+如果您能提供更多详细信息（例如具体的科目分数分布情况），我可以帮助您更准确地判断您的录取可能性。同时，请访问 [https://ipsi.deu.ac.kr/main.do](https://ipsi.deu.ac.kr/main.do) 获取最新的官方信息和具体要求。</t>
+        </is>
+      </c>
+      <c r="D366" t="n">
+        <v>0.1197388567872219</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>동의대학교 화학환경공학부의 수능 일반학생전형 최초합격자 데이터를 바탕으로 판단해보겠습니다.
+- 국어 + 수학 + 탐구(2개) (가산점 포함) 표준 변환 점수 합 평균: 276.61
+- 영어 등급 평균: 4.70
+- 수능 4개 영역 등급 평균: 5.59
+- 수능 4개 영역 (가산점 포함) 표준 변환 점수 합 평균: 385.99
+귀하의 성적 4.25는 최초합격자의 평균값보다 높으므로 합격 가능성이 높은 것으로 판단됩니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>2024년 동의대학교 화학공학과(화학공학과 - 교직)는 공과대학에 속해 있으며, 해당 학과의 모집인원은 43명입니다. 수능 일반학생전형으로 지원할 경우, 수능 성적만을 기준으로 합격 여부를 결정합니다.
+수능 성적 반영 비율은 100%이며, 수능 점수는 국어, 수학(미적분 또는 기하), 영어 등급에 따른 점수 등을 종합적으로 평가하게 됩니다. 따라서, 정시 성적 4.25를 화학공학과의 수능 최소 합격 점수와 비교하여 판단해야 합니다.
+일반적으로, 동의대학교 화학공학과의 수능 최소 합격 점수가 공개되지 않기 때문에, 정확한 정보를 얻으려면 동의대학교 입학처 웹사이트나 전화로 문의하시는 것이 좋습니다. 하지만 일반적인 기준으로 보면, 4.25는 좋은 성적입니다.
+만약 해당 학과의 수능 최소 합격 점수가 4.0 이상이라면, 4.25는 충분히 경쟁력을 갖춘 점수로 볼 수 있습니다. 그러나 정확한 정보를 얻기 위해서는 동의대학교 입학처에 직접 문의하시는 것이 가장 좋습니다.
+추가적으로, 지원자의 전형 요소(학생부 성적, 면접 등)도 합격 여부에 영향을 미칠 수 있으므로, 모든 지원자들이 동일한 기준으로 평가되는 것은 아닙니다.</t>
+        </is>
+      </c>
+      <c r="D367" t="n">
+        <v>0.127136582320319</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>영화학과의 2024학년도 수능(일반학생전형) 최종등록자의 평균 성적을 보면 다음과 같습니다:
+- 국어 + 수학 + 탐구(2개) (가산점 포함) 표준 변환 점수 합: 286.77 (표준 편차: 17.29)
+- 영어 등급: 3.66 (표준 편차: 1.24)
+- 수능 4개 영역 등급: 5.04 (표준 편차: 0.76)
+- 수능 4개 영역 (가산점 포함) 표준 변환 점수 합: 404.43 (표준 편차: 27.09)
+이를 통해, 귀하의 정시 성적이 4.2정도라면 영화학과에 합격할 가능성이 존재한다고 판단됩니다.
+자세한 사항은 "https://ipsi.deu.ac.kr/main.do"에서 확인하시기 바랍니다.</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>4.2라는 점수는 일반적으로 좋은 성적입니다만, 실제 합격 가능성은 여러 요소에 따라 달라질 수 있습니다.
+1. **전형 방식**: 영화학과의 정시 전형 방식을 확인해야 합니다. 만약 나군(일반학생전형)이라면, 수능 4개 영역 중 상위 3개 영역의 표준점수 및 등급점수를 합산한 점수 ÷ 2가 반영됩니다.
+2. **성적 산출**: 
+   - 국어, 수학, 영어, 탐구 중 상위 3개 영역을 선택하여 평균을 구합니다.
+   - 예를 들어, 국어: 90점, 수학: 85점, 영어: 75점, 탐구: 65점이라면 (90 + 85 + 75) / 3 = 80점이 됩니다.
+3. **경쟁률**: 영화학과의 경쟁률을 확인해야 합니다. 경쟁률이 높다면, 평균적인 점수보다 조금 더 높은 점수가 필요할 수 있습니다.
+4. **추가 요소**: 일부 학교에서는 면접이나 서류평가 등 추가 요소를 고려하기도 하므로, 이 부분을 참고해야 합니다.
+5. **대학별 차이**: 각 대학마다 전형 방식과 기준이 다릅니다. 따라서, 해당 대학의 정시 전형 방식을 꼭 확인해보세요.
+만약 영화학과가 나군(일반학생전형)이라면, 4.2라는 점수는 상위권에 속합니다. 그러나 경쟁률이 높다면, 조금 더 높은 점수가 필요할 수 있습니다. 따라서 최종 합격 가능성은 정확한 정보를 바탕으로 판단해야 합니다.
+추가적으로, 대학의 공식 홈페이지나 입학처와 연락하여 자세한 정보를 확인하는 것이 좋습니다.</t>
+        </is>
+      </c>
+      <c r="D368" t="n">
+        <v>0.1267610464503329</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>면접 절차는 다음과 같습니다:
+1. 대기실 입실
+2. 신분 확인
+3. 고사장 앞 이동
+4. 고사장 입실
+5. 지원동기 및 학업계획 발표
+6. 학업역량, 전공적합성 관련 공통문항 발표 및 질의응답
+7. 기타 질의응답(제출서류 진위 여부 등)
+8. 퇴실</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>면접 절차는 다음과 같습니다:
+1. 대기실 입실
+2. 신분 확인
+3. 고사장 앞 이동
+4. 고사장 입실
+5. 지원동기 및 학업계획 발표
+6. 학업역량, 전공적합성 관련 공통문항 발표 및 질의응답
+7. 기타 질의응답 (제출서류 진위 여부 등)
+8. 퇴실
+이 절차는 모든 면접 참여자가 동일하게 진행되며, 블라인드 면접 방식으로 진행됩니다. 즉, 면접위원들은 수험생의 개인 정보를 알 수 없습니다.</t>
+        </is>
+      </c>
+      <c r="D369" t="n">
+        <v>0.5885728063511493</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>GPT-4o-mini Average</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D370" t="n">
+        <v>0.3280925695162146</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>Google Gemma-2-9b-it Average</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D371" t="n">
+        <v>0.2682980797791024</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>Meta Llama-3.1-Instruct Average</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D372" t="n">
+        <v>0.09430187624113912</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>Qwen2.5-7B-instruct Average</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D373" t="n">
+        <v>0.2204960806228673</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
           <t>Total Average</t>
         </is>
       </c>
-      <c r="B273" t="inlineStr">
+      <c r="B374" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="C273" t="inlineStr">
+      <c r="C374" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="D273" t="n">
-        <v>0.2464611660967506</v>
+      <c r="D374" t="n">
+        <v>0.2394054363484127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>